<commit_message>
macro as separate txt file
</commit_message>
<xml_diff>
--- a/parameter_manager.xlsx
+++ b/parameter_manager.xlsx
@@ -406,7 +406,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -435,22 +435,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -479,7 +467,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -489,10 +477,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -578,8 +562,8 @@
   </sheetPr>
   <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -696,7 +680,7 @@
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="7" t="n">
+      <c r="B13" s="2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -704,7 +688,7 @@
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="8" t="n">
+      <c r="B14" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -713,7 +697,7 @@
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="7" t="n">
+      <c r="B15" s="2" t="n">
         <v>100</v>
       </c>
     </row>
@@ -721,7 +705,7 @@
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="9" t="n">
+      <c r="B16" s="7" t="n">
         <v>1E-008</v>
       </c>
     </row>
@@ -729,7 +713,7 @@
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="7" t="n">
+      <c r="B17" s="2" t="n">
         <v>10</v>
       </c>
     </row>
@@ -737,7 +721,7 @@
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="7" t="n">
+      <c r="B18" s="2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -745,7 +729,7 @@
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="8" t="n">
+      <c r="B19" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -754,7 +738,7 @@
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="8" t="n">
+      <c r="B20" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -763,7 +747,7 @@
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="7" t="n">
+      <c r="B21" s="2" t="n">
         <v>0.004</v>
       </c>
     </row>
@@ -771,7 +755,7 @@
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="8" t="n">
+      <c r="B22" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -780,7 +764,7 @@
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="7" t="n">
+      <c r="B23" s="2" t="n">
         <v>2</v>
       </c>
     </row>
@@ -788,7 +772,7 @@
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="7" t="n">
+      <c r="B24" s="2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -796,7 +780,7 @@
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="7" t="n">
+      <c r="B25" s="2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -804,7 +788,7 @@
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="8" t="n">
+      <c r="B26" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -813,7 +797,7 @@
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="8" t="n">
+      <c r="B27" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -830,7 +814,7 @@
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="10" t="n">
+      <c r="B29" s="7" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -838,16 +822,16 @@
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="10"/>
+      <c r="B30" s="7"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="10"/>
+      <c r="B31" s="7"/>
     </row>
     <row r="32" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="12"/>
+      <c r="B32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
@@ -878,7 +862,7 @@
       <c r="A36" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="10" t="n">
+      <c r="B36" s="7" t="n">
         <v>207000</v>
       </c>
     </row>
@@ -890,11 +874,11 @@
         <v>0.29</v>
       </c>
     </row>
-    <row r="38" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="13" t="s">
+    <row r="38" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B38" s="14"/>
+      <c r="B38" s="11"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
@@ -916,7 +900,7 @@
       <c r="A41" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B41" s="10" t="n">
+      <c r="B41" s="7" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -924,7 +908,7 @@
       <c r="A42" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="16" t="n">
+      <c r="B42" s="13" t="n">
         <v>16.93</v>
       </c>
     </row>
@@ -1019,11 +1003,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="13" t="s">
+    <row r="52" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B52" s="14"/>
+      <c r="B52" s="11"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
@@ -1108,10 +1092,10 @@
       <c r="B63" s="6"/>
     </row>
     <row r="64" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="11" t="s">
+      <c r="A64" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B64" s="12"/>
+      <c r="B64" s="9"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
@@ -1183,10 +1167,10 @@
       </c>
     </row>
     <row r="75" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="11" t="s">
+      <c r="A75" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B75" s="12"/>
+      <c r="B75" s="9"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
@@ -1303,7 +1287,7 @@
       <c r="A89" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B89" s="7" t="n">
+      <c r="B89" s="2" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1338,110 +1322,111 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="40.22"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="17" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="40.22"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="14" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="18" t="str">
+      <c r="B1" s="15" t="str">
         <f aca="false">Sheet1!B1</f>
         <v>Qplate</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="str">
+      <c r="A2" s="14" t="str">
         <f aca="false">Sheet1!A2</f>
         <v>#export column marked by “x”</v>
       </c>
-      <c r="B2" s="17" t="str">
+      <c r="B2" s="14" t="str">
         <f aca="false">Sheet1!B2</f>
         <v>x</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="str">
+      <c r="A3" s="14" t="str">
         <f aca="false">Sheet1!A3</f>
         <v># Legend: Qplate-</v>
       </c>
-      <c r="B3" s="17" t="str">
+      <c r="B3" s="14" t="str">
         <f aca="false">Sheet1!B3</f>
         <v>aniso</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="str">
+      <c r="A4" s="14" t="str">
         <f aca="false">Sheet1!A4</f>
         <v>##start</v>
       </c>
     </row>
-    <row r="5" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19" t="str">
+    <row r="5" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="16" t="str">
         <f aca="false">Sheet1!A5</f>
         <v>#subsection General</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="str">
+      <c r="A6" s="14" t="str">
         <f aca="false">Sheet1!A6</f>
         <v>Number of adaptive refinements</v>
       </c>
-      <c r="B6" s="20" t="n">
+      <c r="B6" s="17" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="str">
+      <c r="A7" s="14" t="str">
         <f aca="false">Sheet1!$A$7</f>
         <v>Max refinement level</v>
       </c>
-      <c r="B7" s="20" t="n">
+      <c r="B7" s="17" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="21" t="str">
+      <c r="A8" s="14" t="str">
         <f aca="false">Sheet1!$A$8</f>
         <v>Number global refinements</v>
       </c>
-      <c r="B8" s="20" t="n">
+      <c r="B8" s="17" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="str">
+      <c r="A9" s="14" t="str">
         <f aca="false">Sheet1!$A$9</f>
         <v>Apply global refinements stepwise</v>
       </c>
-      <c r="B9" s="22" t="b">
+      <c r="B9" s="18" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17" t="str">
+      <c r="A10" s="14" t="str">
         <f aca="false">Sheet1!$A$10</f>
         <v>AMR afresh on new meshes</v>
       </c>
-      <c r="B10" s="22" t="n">
+      <c r="B10" s="18" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="str">
+      <c r="A11" s="14" t="str">
         <f aca="false">Sheet1!$A$11</f>
         <v>Input for the KellyErrorEstimator</v>
       </c>
-      <c r="B11" s="20" t="n">
+      <c r="B11" s="17" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IRV: different prm set
</commit_message>
<xml_diff>
--- a/parameter_manager.xlsx
+++ b/parameter_manager.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="98">
   <si>
     <t xml:space="preserve">Qplate</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t xml:space="preserve">tensileSpecimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TenSpec-dmg</t>
   </si>
   <si>
     <t xml:space="preserve">##start</t>
@@ -421,7 +424,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -500,6 +503,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -613,8 +620,8 @@
   </sheetPr>
   <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -646,7 +653,7 @@
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="0"/>
@@ -673,16 +680,19 @@
       <c r="G3" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="H3" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4"/>
     </row>
     <row r="5" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="5"/>
       <c r="D5" s="7"/>
@@ -691,7 +701,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>0</v>
@@ -706,12 +716,15 @@
         <v>0</v>
       </c>
       <c r="G6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>100</v>
@@ -728,10 +741,13 @@
       <c r="G7" s="8" t="n">
         <v>100</v>
       </c>
+      <c r="H7" s="8" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>2</v>
@@ -748,10 +764,13 @@
       <c r="G8" s="8" t="n">
         <v>1</v>
       </c>
+      <c r="H8" s="8" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -770,13 +789,17 @@
         <v>0</v>
       </c>
       <c r="G9" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -795,13 +818,17 @@
         <v>0</v>
       </c>
       <c r="G10" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>0</v>
@@ -816,18 +843,21 @@
         <v>1</v>
       </c>
       <c r="G11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D12" s="8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="3" t="n">
         <v>0</v>
@@ -837,11 +867,14 @@
       </c>
       <c r="G12" s="8" t="n">
         <v>0</v>
+      </c>
+      <c r="H12" s="8" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>1</v>
@@ -857,11 +890,14 @@
       </c>
       <c r="G13" s="8" t="n">
         <v>1</v>
+      </c>
+      <c r="H13" s="8" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -880,13 +916,17 @@
         <v>0</v>
       </c>
       <c r="G14" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>100</v>
@@ -903,10 +943,13 @@
       <c r="G15" s="8" t="n">
         <v>100</v>
       </c>
+      <c r="H15" s="8" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B16" s="10" t="n">
         <v>1E-008</v>
@@ -923,10 +966,13 @@
       <c r="G16" s="11" t="n">
         <v>1E-008</v>
       </c>
+      <c r="H16" s="11" t="n">
+        <v>1E-008</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>10</v>
@@ -941,12 +987,15 @@
         <v>10</v>
       </c>
       <c r="G17" s="8" t="n">
-        <v>20</v>
+        <v>10</v>
+      </c>
+      <c r="H17" s="8" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18" s="2" t="n">
         <v>1</v>
@@ -961,12 +1010,15 @@
         <v>1</v>
       </c>
       <c r="G18" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" s="8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B19" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -985,13 +1037,17 @@
         <v>0</v>
       </c>
       <c r="G19" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B20" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -1010,13 +1066,17 @@
         <v>0</v>
       </c>
       <c r="G20" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21" s="2" t="n">
         <v>0.004</v>
@@ -1025,18 +1085,22 @@
         <v>0.004</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>0.0001</v>
+        <f aca="false">0.015/100</f>
+        <v>0.00015</v>
       </c>
       <c r="F21" s="3" t="n">
         <v>0.001</v>
       </c>
       <c r="G21" s="8" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H21" s="8" t="n">
         <v>0.01</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B22" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -1055,13 +1119,17 @@
         <v>0</v>
       </c>
       <c r="G22" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B23" s="2" t="n">
         <v>2</v>
@@ -1076,12 +1144,15 @@
         <v>2</v>
       </c>
       <c r="G23" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="H23" s="8" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B24" s="2" t="n">
         <v>1</v>
@@ -1096,12 +1167,15 @@
         <v>2</v>
       </c>
       <c r="G24" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H24" s="3" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B25" s="2" t="n">
         <v>1</v>
@@ -1118,10 +1192,13 @@
       <c r="G25" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="H25" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B26" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -1140,24 +1217,29 @@
         <v>0</v>
       </c>
       <c r="G26" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B27" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D27" s="9" t="b">
-        <v>0</v>
+      <c r="D27" s="9" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="E27" s="9" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="F27" s="9" t="n">
         <f aca="false">FALSE()</f>
@@ -1167,10 +1249,14 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="H27" s="9" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B28" s="2" t="n">
         <v>0.007</v>
@@ -1185,12 +1271,15 @@
         <v>0.0003</v>
       </c>
       <c r="G28" s="8" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
+      </c>
+      <c r="H28" s="8" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B29" s="10" t="n">
         <v>1E-006</v>
@@ -1207,10 +1296,13 @@
       <c r="G29" s="11" t="n">
         <v>1E-006</v>
       </c>
+      <c r="H29" s="11" t="n">
+        <v>1E-006</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B30" s="10"/>
     </row>
@@ -1219,7 +1311,7 @@
     </row>
     <row r="32" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B32" s="14"/>
       <c r="D32" s="7"/>
@@ -1228,7 +1320,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B33" s="2" t="n">
         <v>2</v>
@@ -1237,7 +1329,7 @@
         <v>4</v>
       </c>
       <c r="E33" s="3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F33" s="3" t="n">
         <v>5</v>
@@ -1245,10 +1337,13 @@
       <c r="G33" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="H33" s="8" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B34" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -1267,13 +1362,17 @@
         <v>1</v>
       </c>
       <c r="G34" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H34" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B35" s="2" t="n">
         <v>0</v>
@@ -1288,12 +1387,15 @@
         <v>0</v>
       </c>
       <c r="G35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" s="8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B36" s="10" t="n">
         <v>207000</v>
@@ -1302,18 +1404,21 @@
         <v>207000</v>
       </c>
       <c r="E36" s="11" t="n">
-        <v>207000</v>
+        <v>210000</v>
       </c>
       <c r="F36" s="12" t="n">
         <v>207000</v>
       </c>
       <c r="G36" s="11" t="n">
-        <v>207000</v>
+        <v>210000</v>
+      </c>
+      <c r="H36" s="11" t="n">
+        <v>210000</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B37" s="2" t="n">
         <v>0.29</v>
@@ -1322,18 +1427,21 @@
         <v>0.29</v>
       </c>
       <c r="E37" s="8" t="n">
-        <v>0.29</v>
+        <v>0.3</v>
       </c>
       <c r="F37" s="3" t="n">
         <v>0.3</v>
       </c>
       <c r="G37" s="8" t="n">
-        <v>0.29</v>
+        <v>0.3</v>
+      </c>
+      <c r="H37" s="8" t="n">
+        <v>0.3</v>
       </c>
     </row>
     <row r="38" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B38" s="17"/>
       <c r="D38" s="19"/>
@@ -1342,7 +1450,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B39" s="2" t="n">
         <v>0</v>
@@ -1351,18 +1459,21 @@
         <v>0</v>
       </c>
       <c r="E39" s="3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F39" s="3" t="n">
         <v>0</v>
       </c>
       <c r="G39" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H39" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B40" s="2" t="n">
         <v>40</v>
@@ -1371,18 +1482,21 @@
         <v>40</v>
       </c>
       <c r="E40" s="3" t="n">
-        <v>40</v>
+        <v>375.7133</v>
       </c>
       <c r="F40" s="12" t="n">
         <v>40</v>
       </c>
-      <c r="G40" s="0" t="n">
-        <v>450</v>
+      <c r="G40" s="20" t="n">
+        <v>375.7133</v>
+      </c>
+      <c r="H40" s="20" t="n">
+        <v>375.7133</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B41" s="10" t="n">
         <v>1000</v>
@@ -1391,32 +1505,45 @@
         <v>1000</v>
       </c>
       <c r="E41" s="12" t="n">
-        <v>2000</v>
+        <v>133.59798</v>
       </c>
       <c r="F41" s="12" t="n">
         <v>2000</v>
       </c>
       <c r="G41" s="11" t="n">
-        <v>1000</v>
+        <v>133.598</v>
+      </c>
+      <c r="H41" s="11" t="n">
+        <f aca="false">+1000/1.5</f>
+        <v>666.666666666667</v>
+      </c>
+      <c r="I41" s="11" t="n">
+        <v>133.598</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B42" s="20" t="n">
+        <v>48</v>
+      </c>
+      <c r="B42" s="21" t="n">
         <v>16.93</v>
       </c>
-      <c r="D42" s="21" t="n">
+      <c r="D42" s="22" t="n">
         <v>16.93</v>
       </c>
-      <c r="G42" s="21" t="n">
-        <v>16.93</v>
+      <c r="E42" s="3" t="n">
+        <v>19.9999915</v>
+      </c>
+      <c r="G42" s="22" t="n">
+        <v>19.99999</v>
+      </c>
+      <c r="H42" s="22" t="n">
+        <v>19.99999</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B43" s="2" t="n">
         <v>265</v>
@@ -1425,18 +1552,21 @@
         <v>265</v>
       </c>
       <c r="E43" s="3" t="n">
-        <v>10</v>
+        <v>357.18534</v>
       </c>
       <c r="F43" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="G43" s="8" t="n">
-        <v>265</v>
+      <c r="G43" s="11" t="n">
+        <v>357.1853</v>
+      </c>
+      <c r="H43" s="11" t="n">
+        <v>357.1853</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B44" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -1458,10 +1588,14 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="H44" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B45" s="2" t="n">
         <v>1.25</v>
@@ -1475,10 +1609,13 @@
       <c r="G45" s="8" t="n">
         <v>1.25</v>
       </c>
+      <c r="H45" s="8" t="n">
+        <v>1.25</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B46" s="2" t="n">
         <v>0.75</v>
@@ -1492,10 +1629,13 @@
       <c r="G46" s="8" t="n">
         <v>0.75</v>
       </c>
+      <c r="H46" s="8" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B47" s="2" t="n">
         <v>1</v>
@@ -1507,12 +1647,15 @@
         <v>1</v>
       </c>
       <c r="G47" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H47" s="8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B48" s="2" t="n">
         <v>0.4</v>
@@ -1526,10 +1669,13 @@
       <c r="G48" s="8" t="n">
         <v>0.4</v>
       </c>
+      <c r="H48" s="8" t="n">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B49" s="2" t="n">
         <v>0.4</v>
@@ -1543,10 +1689,13 @@
       <c r="G49" s="8" t="n">
         <v>0.4</v>
       </c>
+      <c r="H49" s="8" t="n">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B50" s="2" t="n">
         <v>0.4</v>
@@ -1560,10 +1709,13 @@
       <c r="G50" s="8" t="n">
         <v>0.4</v>
       </c>
+      <c r="H50" s="8" t="n">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B51" s="2" t="n">
         <v>0</v>
@@ -1572,21 +1724,24 @@
         <v>0</v>
       </c>
       <c r="G51" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" s="8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="52" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B52" s="17"/>
-      <c r="D52" s="22"/>
+      <c r="D52" s="23"/>
       <c r="E52" s="19"/>
       <c r="F52" s="19"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B53" s="2" t="n">
         <v>1</v>
@@ -1601,12 +1756,15 @@
         <v>1</v>
       </c>
       <c r="G53" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H53" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B54" s="2" t="n">
         <v>2</v>
@@ -1623,13 +1781,16 @@
       <c r="G54" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="H54" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D55" s="3" t="n">
         <v>1</v>
@@ -1643,10 +1804,13 @@
       <c r="G55" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="H55" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B56" s="2" t="n">
         <v>10</v>
@@ -1663,13 +1827,16 @@
       <c r="G56" s="12" t="n">
         <v>1000000</v>
       </c>
+      <c r="H56" s="12" t="n">
+        <v>1000000</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D57" s="3" t="n">
         <v>0.4</v>
@@ -1683,13 +1850,16 @@
       <c r="G57" s="3" t="n">
         <v>0.4</v>
       </c>
+      <c r="H57" s="3" t="n">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D58" s="8" t="n">
         <v>0.008</v>
@@ -1703,10 +1873,16 @@
       <c r="G58" s="8" t="n">
         <v>0.008</v>
       </c>
+      <c r="H58" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I58" s="0" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B59" s="2" t="n">
         <v>3</v>
@@ -1723,10 +1899,13 @@
       <c r="G59" s="8" t="n">
         <v>3</v>
       </c>
+      <c r="H59" s="8" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B60" s="2" t="n">
         <v>10</v>
@@ -1743,10 +1922,13 @@
       <c r="G60" s="8" t="n">
         <v>10</v>
       </c>
+      <c r="H60" s="8" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B61" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -1765,13 +1947,17 @@
         <v>0</v>
       </c>
       <c r="G61" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H61" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D62" s="8"/>
     </row>
@@ -1780,16 +1966,16 @@
     </row>
     <row r="64" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B64" s="14"/>
-      <c r="D64" s="23"/>
+      <c r="D64" s="24"/>
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B65" s="2" t="n">
         <v>100</v>
@@ -1804,12 +1990,15 @@
         <v>1</v>
       </c>
       <c r="G65" s="0" t="n">
-        <v>50</v>
+        <v>40</v>
+      </c>
+      <c r="H65" s="0" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B66" s="2" t="n">
         <v>50</v>
@@ -1820,10 +2009,13 @@
       <c r="G66" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="H66" s="0" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B67" s="2" t="n">
         <v>20</v>
@@ -1834,21 +2026,24 @@
       <c r="G67" s="0" t="n">
         <v>1.5</v>
       </c>
+      <c r="H67" s="0" t="n">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B69" s="2" t="n">
         <v>1</v>
@@ -1859,10 +2054,13 @@
       <c r="G69" s="0" t="n">
         <v>25</v>
       </c>
+      <c r="H69" s="0" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B70" s="2" t="n">
         <v>8.98</v>
@@ -1873,10 +2071,13 @@
       <c r="G70" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="H70" s="0" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B71" s="2" t="n">
         <v>3</v>
@@ -1887,10 +2088,13 @@
       <c r="G71" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="H71" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B72" s="2" t="n">
         <v>8</v>
@@ -1901,7 +2105,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D73" s="8"/>
     </row>
@@ -1910,16 +2114,16 @@
     </row>
     <row r="75" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B75" s="14"/>
-      <c r="D75" s="23"/>
+      <c r="D75" s="24"/>
       <c r="E75" s="7"/>
       <c r="F75" s="7"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B76" s="2" t="n">
         <v>1</v>
@@ -1928,12 +2132,15 @@
         <v>1</v>
       </c>
       <c r="G76" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H76" s="8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B77" s="2" t="n">
         <v>1</v>
@@ -1942,12 +2149,15 @@
         <v>1</v>
       </c>
       <c r="G77" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H77" s="8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B78" s="2" t="n">
         <v>1</v>
@@ -1956,12 +2166,15 @@
         <v>1</v>
       </c>
       <c r="G78" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H78" s="8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B79" s="2" t="n">
         <v>1</v>
@@ -1970,21 +2183,27 @@
         <v>1</v>
       </c>
       <c r="G79" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H79" s="8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D80" s="8"/>
       <c r="G80" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="H80" s="0" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B81" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -2006,10 +2225,14 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="H81" s="9" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B82" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -2028,13 +2251,17 @@
         <v>0</v>
       </c>
       <c r="G82" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H82" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B83" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -2053,13 +2280,17 @@
         <v>0</v>
       </c>
       <c r="G83" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H83" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B84" s="2" t="n">
         <v>2</v>
@@ -2067,19 +2298,22 @@
       <c r="D84" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="E84" s="3" t="n">
+      <c r="E84" s="8" t="n">
         <v>2</v>
       </c>
       <c r="F84" s="8" t="n">
         <v>2</v>
       </c>
       <c r="G84" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="H84" s="8" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B85" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -2098,13 +2332,17 @@
         <v>0</v>
       </c>
       <c r="G85" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H85" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B86" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -2123,13 +2361,17 @@
         <v>0</v>
       </c>
       <c r="G86" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H86" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B87" s="2" t="n">
         <v>0</v>
@@ -2137,19 +2379,22 @@
       <c r="D87" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="E87" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F87" s="3" t="n">
+      <c r="E87" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F87" s="8" t="n">
         <v>0</v>
       </c>
       <c r="G87" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H87" s="8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B88" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -2171,10 +2416,14 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="H88" s="9" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B89" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -2196,10 +2445,14 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="H89" s="9" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B90" s="2" t="n">
         <v>2</v>
@@ -2214,17 +2467,20 @@
         <v>2</v>
       </c>
       <c r="G90" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="H90" s="8" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2254,105 +2510,105 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="40.22"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="24" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="40.22"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="25" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="25" t="str">
+      <c r="B1" s="26" t="str">
         <f aca="false">Sheet1!B1</f>
         <v>Qplate</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="str">
+      <c r="A2" s="25" t="str">
         <f aca="false">Sheet1!A2</f>
         <v>#export column marked by “x”</v>
       </c>
-      <c r="B2" s="24" t="n">
+      <c r="B2" s="25" t="n">
         <f aca="false">Sheet1!B2</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="str">
+      <c r="A3" s="25" t="str">
         <f aca="false">Sheet1!A3</f>
         <v># Legend: _</v>
       </c>
-      <c r="B3" s="24" t="str">
+      <c r="B3" s="25" t="str">
         <f aca="false">Sheet1!B3</f>
         <v>Qplate-2D-aniso</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="str">
+      <c r="A4" s="25" t="str">
         <f aca="false">Sheet1!A4</f>
         <v>##start</v>
       </c>
     </row>
-    <row r="5" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="26" t="str">
+    <row r="5" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="27" t="str">
         <f aca="false">Sheet1!A5</f>
         <v>#subsection General</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24" t="str">
+      <c r="A6" s="25" t="str">
         <f aca="false">Sheet1!A6</f>
         <v>Number of adaptive refinements</v>
       </c>
-      <c r="B6" s="27" t="n">
+      <c r="B6" s="28" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24" t="str">
+      <c r="A7" s="25" t="str">
         <f aca="false">Sheet1!$A$7</f>
         <v>Max refinement level</v>
       </c>
-      <c r="B7" s="27" t="n">
+      <c r="B7" s="28" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="24" t="str">
+      <c r="A8" s="25" t="str">
         <f aca="false">Sheet1!$A$8</f>
         <v>Number global refinements</v>
       </c>
-      <c r="B8" s="27" t="n">
+      <c r="B8" s="28" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="24" t="str">
+      <c r="A9" s="25" t="str">
         <f aca="false">Sheet1!$A$9</f>
         <v>Apply global refinements stepwise</v>
       </c>
-      <c r="B9" s="27" t="n">
+      <c r="B9" s="28" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="24" t="str">
+      <c r="A10" s="25" t="str">
         <f aca="false">Sheet1!$A$10</f>
         <v>AMR afresh on new meshes</v>
       </c>
-      <c r="B10" s="27" t="n">
+      <c r="B10" s="28" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="24" t="str">
+      <c r="A11" s="25" t="str">
         <f aca="false">Sheet1!$A$11</f>
         <v>Input for the KellyErrorEstimator</v>
       </c>
-      <c r="B11" s="27" t="n">
+      <c r="B11" s="28" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added SheStrip-AMR and QPlate-AMR for adaptivity
</commit_message>
<xml_diff>
--- a/parameter_manager.xlsx
+++ b/parameter_manager.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Guide" sheetId="1" state="visible" r:id="rId2"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="209">
   <si>
     <t xml:space="preserve">#export column marked by “x”</t>
   </si>
@@ -421,7 +421,7 @@
     <t xml:space="preserve">Seupel_etal_2D</t>
   </si>
   <si>
-    <t xml:space="preserve">1D_bar</t>
+    <t xml:space="preserve">SheStrip-AMR</t>
   </si>
   <si>
     <t xml:space="preserve">Anand_etal_8.5</t>
@@ -587,6 +587,9 @@
   </si>
   <si>
     <t xml:space="preserve">2D_GPD-Phid_alpha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QPlate-AMR</t>
   </si>
   <si>
     <t xml:space="preserve">0.4</t>
@@ -959,7 +962,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1106,6 +1109,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1363,9 +1370,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>95760</xdr:colOff>
+      <xdr:colOff>95040</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>123120</xdr:rowOff>
+      <xdr:rowOff>122400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1375,7 +1382,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1000800" y="2806920"/>
-          <a:ext cx="5597280" cy="2680560"/>
+          <a:ext cx="5596560" cy="2679840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1474,9 +1481,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>147600</xdr:colOff>
+      <xdr:colOff>146880</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>3600</xdr:rowOff>
+      <xdr:rowOff>2880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1486,7 +1493,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1052640" y="693360"/>
-          <a:ext cx="5597280" cy="773280"/>
+          <a:ext cx="5596560" cy="772560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1537,9 +1544,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
+      <xdr:colOff>136440</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>46800</xdr:rowOff>
+      <xdr:rowOff>46080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1549,7 +1556,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1042200" y="1711800"/>
-          <a:ext cx="5597280" cy="773280"/>
+          <a:ext cx="5596560" cy="772560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1600,9 +1607,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>84960</xdr:colOff>
+      <xdr:colOff>84240</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>144360</xdr:rowOff>
+      <xdr:rowOff>143640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1612,7 +1619,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="990000" y="5710680"/>
-          <a:ext cx="5597280" cy="773280"/>
+          <a:ext cx="5596560" cy="772560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1728,19 +1735,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="22" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
       <c r="F1" s="22"/>
       <c r="G1" s="22" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I1" s="22"/>
     </row>
@@ -1759,39 +1766,39 @@
         <v># Legend: _</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
       <c r="G3" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="J3" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="K3" s="46" t="s">
+      <c r="J3" s="47" t="s">
         <v>202</v>
       </c>
-      <c r="L3" s="46" t="s">
+      <c r="K3" s="47" t="s">
         <v>203</v>
       </c>
-      <c r="M3" s="46" t="s">
+      <c r="L3" s="47" t="s">
         <v>204</v>
       </c>
-      <c r="N3" s="46" t="s">
-        <v>203</v>
-      </c>
-      <c r="O3" s="46"/>
+      <c r="M3" s="47" t="s">
+        <v>205</v>
+      </c>
+      <c r="N3" s="47" t="s">
+        <v>204</v>
+      </c>
+      <c r="O3" s="47"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="str">
@@ -2110,7 +2117,7 @@
       <c r="D13" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="E13" s="75"/>
+      <c r="E13" s="76"/>
       <c r="F13" s="8"/>
       <c r="G13" s="26" t="n">
         <v>2</v>
@@ -2187,7 +2194,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="9"/>
-      <c r="F15" s="76"/>
+      <c r="F15" s="77"/>
       <c r="G15" s="26" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -2648,10 +2655,10 @@
         <f aca="false">parameters!A28</f>
         <v>Initial increment</v>
       </c>
-      <c r="B28" s="77" t="n">
+      <c r="B28" s="78" t="n">
         <v>0.01</v>
       </c>
-      <c r="C28" s="77" t="n">
+      <c r="C28" s="78" t="n">
         <v>0.01</v>
       </c>
       <c r="D28" s="8" t="n">
@@ -2659,10 +2666,10 @@
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
-      <c r="G28" s="77" t="n">
+      <c r="G28" s="78" t="n">
         <v>0.01</v>
       </c>
-      <c r="H28" s="77" t="n">
+      <c r="H28" s="78" t="n">
         <v>0.01</v>
       </c>
       <c r="I28" s="8" t="n">
@@ -2942,25 +2949,25 @@
         <f aca="false">parameters!A36</f>
         <v>GG-Mode</v>
       </c>
-      <c r="B36" s="78" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C36" s="78" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D36" s="78" t="n">
+      <c r="B36" s="79" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C36" s="79" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D36" s="79" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
-      <c r="G36" s="78" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H36" s="78" t="n">
+      <c r="G36" s="79" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H36" s="79" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3096,25 +3103,25 @@
       <c r="H39" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="I39" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="J39" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="K39" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="L39" s="56" t="n">
+      <c r="I39" s="57" t="n">
+        <v>1</v>
+      </c>
+      <c r="J39" s="57" t="n">
+        <v>1</v>
+      </c>
+      <c r="K39" s="57" t="n">
+        <v>1</v>
+      </c>
+      <c r="L39" s="57" t="n">
         <v>1</v>
       </c>
       <c r="M39" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="N39" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="O39" s="56"/>
+      <c r="N39" s="57" t="n">
+        <v>1</v>
+      </c>
+      <c r="O39" s="57"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="str">
@@ -3197,25 +3204,25 @@
         <f aca="false">parameters!A44</f>
         <v>Use finite strains</v>
       </c>
-      <c r="B44" s="43" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C44" s="43" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D44" s="43" t="n">
+      <c r="B44" s="44" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C44" s="44" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D44" s="44" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E44" s="9"/>
       <c r="F44" s="16"/>
-      <c r="G44" s="43" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H44" s="43" t="n">
+      <c r="G44" s="44" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H44" s="44" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3235,7 +3242,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="M44" s="67" t="n">
+      <c r="M44" s="68" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3371,7 +3378,7 @@
       <c r="O47" s="8"/>
     </row>
     <row r="48" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="73" t="str">
+      <c r="A48" s="74" t="str">
         <f aca="false">parameters!A48</f>
         <v>// plasticity parameters</v>
       </c>
@@ -3646,7 +3653,7 @@
         <v>0</v>
       </c>
       <c r="L55" s="8"/>
-      <c r="M55" s="68" t="n">
+      <c r="M55" s="69" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3788,16 +3795,16 @@
       </c>
     </row>
     <row r="63" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="73" t="str">
+      <c r="A63" s="74" t="str">
         <f aca="false">parameters!A63</f>
         <v>// damage parameters</v>
       </c>
-      <c r="B63" s="48"/>
-      <c r="C63" s="48"/>
-      <c r="D63" s="48"/>
-      <c r="G63" s="48"/>
-      <c r="H63" s="48"/>
-      <c r="I63" s="48"/>
+      <c r="B63" s="49"/>
+      <c r="C63" s="49"/>
+      <c r="D63" s="49"/>
+      <c r="G63" s="49"/>
+      <c r="H63" s="49"/>
+      <c r="I63" s="49"/>
       <c r="AMH63" s="0"/>
       <c r="AMI63" s="0"/>
       <c r="AMJ63" s="0"/>
@@ -4114,10 +4121,10 @@
       <c r="G74" s="11"/>
       <c r="H74" s="11"/>
       <c r="I74" s="8"/>
-      <c r="J74" s="66" t="n">
+      <c r="J74" s="67" t="n">
         <v>1000</v>
       </c>
-      <c r="K74" s="66" t="n">
+      <c r="K74" s="67" t="n">
         <v>1000</v>
       </c>
       <c r="L74" s="35" t="n">
@@ -4181,12 +4188,12 @@
         <f aca="false">parameters!A79</f>
         <v>#subsection Geometry</v>
       </c>
-      <c r="B79" s="49"/>
-      <c r="C79" s="49"/>
-      <c r="D79" s="49"/>
-      <c r="G79" s="49"/>
-      <c r="H79" s="49"/>
-      <c r="I79" s="49"/>
+      <c r="B79" s="50"/>
+      <c r="C79" s="50"/>
+      <c r="D79" s="50"/>
+      <c r="G79" s="50"/>
+      <c r="H79" s="50"/>
+      <c r="I79" s="50"/>
       <c r="AMH79" s="0"/>
       <c r="AMI79" s="0"/>
       <c r="AMJ79" s="0"/>
@@ -4468,12 +4475,12 @@
         <f aca="false">parameters!A91</f>
         <v>#subsection Modeling</v>
       </c>
-      <c r="B91" s="49"/>
-      <c r="C91" s="49"/>
-      <c r="D91" s="49"/>
-      <c r="G91" s="49"/>
-      <c r="H91" s="49"/>
-      <c r="I91" s="49"/>
+      <c r="B91" s="50"/>
+      <c r="C91" s="50"/>
+      <c r="D91" s="50"/>
+      <c r="G91" s="50"/>
+      <c r="H91" s="50"/>
+      <c r="I91" s="50"/>
       <c r="AMH91" s="0"/>
       <c r="AMI91" s="0"/>
       <c r="AMJ91" s="0"/>
@@ -5200,7 +5207,7 @@
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="22"/>
       <c r="C1" s="22" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
@@ -5225,16 +5232,16 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="str">
@@ -5466,7 +5473,7 @@
         <f aca="false">parameters!A21</f>
         <v>Max nbr of NR its</v>
       </c>
-      <c r="B21" s="50" t="n">
+      <c r="B21" s="51" t="n">
         <v>200</v>
       </c>
       <c r="C21" s="8"/>
@@ -5622,7 +5629,7 @@
         <f aca="false">parameters!A34</f>
         <v>Numerical Example</v>
       </c>
-      <c r="B34" s="79" t="n">
+      <c r="B34" s="80" t="n">
         <v>10</v>
       </c>
       <c r="C34" s="8"/>
@@ -5744,12 +5751,12 @@
         <f aca="false">parameters!A44</f>
         <v>Use finite strains</v>
       </c>
-      <c r="B44" s="43" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C44" s="43"/>
-      <c r="D44" s="43"/>
+      <c r="B44" s="44" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C44" s="44"/>
+      <c r="D44" s="44"/>
       <c r="E44" s="9"/>
       <c r="F44" s="16"/>
     </row>
@@ -5792,7 +5799,7 @@
       <c r="F47" s="8"/>
     </row>
     <row r="48" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="73" t="str">
+      <c r="A48" s="74" t="str">
         <f aca="false">parameters!A48</f>
         <v>// plasticity parameters</v>
       </c>
@@ -5824,7 +5831,7 @@
         <f aca="false">parameters!A51</f>
         <v>Yield stress</v>
       </c>
-      <c r="B51" s="47" t="n">
+      <c r="B51" s="48" t="n">
         <v>1000000</v>
       </c>
       <c r="C51" s="10"/>
@@ -5960,13 +5967,13 @@
       <c r="F62" s="8"/>
     </row>
     <row r="63" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="73" t="str">
+      <c r="A63" s="74" t="str">
         <f aca="false">parameters!A63</f>
         <v>// damage parameters</v>
       </c>
-      <c r="B63" s="48"/>
-      <c r="C63" s="48"/>
-      <c r="D63" s="48"/>
+      <c r="B63" s="49"/>
+      <c r="C63" s="49"/>
+      <c r="D63" s="49"/>
       <c r="AMH63" s="0"/>
       <c r="AMI63" s="0"/>
       <c r="AMJ63" s="0"/>
@@ -6119,9 +6126,9 @@
         <f aca="false">parameters!A79</f>
         <v>#subsection Geometry</v>
       </c>
-      <c r="B79" s="49"/>
-      <c r="C79" s="49"/>
-      <c r="D79" s="49"/>
+      <c r="B79" s="50"/>
+      <c r="C79" s="50"/>
+      <c r="D79" s="50"/>
       <c r="AMH79" s="0"/>
       <c r="AMI79" s="0"/>
       <c r="AMJ79" s="0"/>
@@ -6226,9 +6233,9 @@
         <f aca="false">parameters!A91</f>
         <v>#subsection Modeling</v>
       </c>
-      <c r="B91" s="49"/>
-      <c r="C91" s="49"/>
-      <c r="D91" s="49"/>
+      <c r="B91" s="50"/>
+      <c r="C91" s="50"/>
+      <c r="D91" s="50"/>
       <c r="AMH91" s="0"/>
       <c r="AMI91" s="0"/>
       <c r="AMJ91" s="0"/>
@@ -6423,7 +6430,7 @@
         <f aca="false">parameters!A106</f>
         <v>Load/displacement control</v>
       </c>
-      <c r="B106" s="79" t="n">
+      <c r="B106" s="80" t="n">
         <v>3</v>
       </c>
       <c r="C106" s="8"/>
@@ -6500,7 +6507,7 @@
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="22"/>
       <c r="C1" s="22" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
@@ -6525,16 +6532,16 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="str">
@@ -6768,7 +6775,7 @@
         <f aca="false">parameters!A21</f>
         <v>Max nbr of NR its</v>
       </c>
-      <c r="B21" s="50" t="n">
+      <c r="B21" s="51" t="n">
         <v>15</v>
       </c>
       <c r="C21" s="8"/>
@@ -6926,7 +6933,7 @@
         <f aca="false">parameters!A34</f>
         <v>Numerical Example</v>
       </c>
-      <c r="B34" s="79" t="n">
+      <c r="B34" s="80" t="n">
         <v>11</v>
       </c>
       <c r="C34" s="8"/>
@@ -7047,12 +7054,12 @@
         <f aca="false">parameters!A44</f>
         <v>Use finite strains</v>
       </c>
-      <c r="B44" s="43" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C44" s="43"/>
-      <c r="D44" s="43"/>
+      <c r="B44" s="44" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C44" s="44"/>
+      <c r="D44" s="44"/>
       <c r="E44" s="9"/>
       <c r="F44" s="16"/>
     </row>
@@ -7095,7 +7102,7 @@
       <c r="F47" s="8"/>
     </row>
     <row r="48" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="73" t="str">
+      <c r="A48" s="74" t="str">
         <f aca="false">parameters!A48</f>
         <v>// plasticity parameters</v>
       </c>
@@ -7127,7 +7134,7 @@
         <f aca="false">parameters!A51</f>
         <v>Yield stress</v>
       </c>
-      <c r="B51" s="47" t="n">
+      <c r="B51" s="48" t="n">
         <v>200</v>
       </c>
       <c r="C51" s="10"/>
@@ -7263,13 +7270,13 @@
       <c r="F62" s="8"/>
     </row>
     <row r="63" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="73" t="str">
+      <c r="A63" s="74" t="str">
         <f aca="false">parameters!A63</f>
         <v>// damage parameters</v>
       </c>
-      <c r="B63" s="48"/>
-      <c r="C63" s="48"/>
-      <c r="D63" s="48"/>
+      <c r="B63" s="49"/>
+      <c r="C63" s="49"/>
+      <c r="D63" s="49"/>
       <c r="AMH63" s="0"/>
       <c r="AMI63" s="0"/>
       <c r="AMJ63" s="0"/>
@@ -7436,9 +7443,9 @@
         <f aca="false">parameters!A79</f>
         <v>#subsection Geometry</v>
       </c>
-      <c r="B79" s="49"/>
-      <c r="C79" s="49"/>
-      <c r="D79" s="49"/>
+      <c r="B79" s="50"/>
+      <c r="C79" s="50"/>
+      <c r="D79" s="50"/>
       <c r="AMH79" s="0"/>
       <c r="AMI79" s="0"/>
       <c r="AMJ79" s="0"/>
@@ -7553,9 +7560,9 @@
         <f aca="false">parameters!A91</f>
         <v>#subsection Modeling</v>
       </c>
-      <c r="B91" s="49"/>
-      <c r="C91" s="49"/>
-      <c r="D91" s="49"/>
+      <c r="B91" s="50"/>
+      <c r="C91" s="50"/>
+      <c r="D91" s="50"/>
       <c r="AMH91" s="0"/>
       <c r="AMI91" s="0"/>
       <c r="AMJ91" s="0"/>
@@ -7827,7 +7834,7 @@
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="22"/>
       <c r="C1" s="22" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
@@ -7852,16 +7859,16 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="str">
@@ -8095,7 +8102,7 @@
         <f aca="false">parameters!A21</f>
         <v>Max nbr of NR its</v>
       </c>
-      <c r="B21" s="50" t="n">
+      <c r="B21" s="51" t="n">
         <v>15</v>
       </c>
       <c r="C21" s="8"/>
@@ -8251,7 +8258,7 @@
         <f aca="false">parameters!A34</f>
         <v>Numerical Example</v>
       </c>
-      <c r="B34" s="79" t="n">
+      <c r="B34" s="80" t="n">
         <v>12</v>
       </c>
       <c r="C34" s="8"/>
@@ -8372,12 +8379,12 @@
         <f aca="false">parameters!A44</f>
         <v>Use finite strains</v>
       </c>
-      <c r="B44" s="43" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C44" s="43"/>
-      <c r="D44" s="43"/>
+      <c r="B44" s="44" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C44" s="44"/>
+      <c r="D44" s="44"/>
       <c r="E44" s="9"/>
       <c r="F44" s="16"/>
     </row>
@@ -8420,7 +8427,7 @@
       <c r="F47" s="8"/>
     </row>
     <row r="48" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="73" t="str">
+      <c r="A48" s="74" t="str">
         <f aca="false">parameters!A48</f>
         <v>// plasticity parameters</v>
       </c>
@@ -8452,7 +8459,7 @@
         <f aca="false">parameters!A51</f>
         <v>Yield stress</v>
       </c>
-      <c r="B51" s="47" t="n">
+      <c r="B51" s="48" t="n">
         <v>20</v>
       </c>
       <c r="C51" s="10"/>
@@ -8586,13 +8593,13 @@
       <c r="F62" s="8"/>
     </row>
     <row r="63" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="73" t="str">
+      <c r="A63" s="74" t="str">
         <f aca="false">parameters!A63</f>
         <v>// damage parameters</v>
       </c>
-      <c r="B63" s="48"/>
-      <c r="C63" s="48"/>
-      <c r="D63" s="48"/>
+      <c r="B63" s="49"/>
+      <c r="C63" s="49"/>
+      <c r="D63" s="49"/>
       <c r="AMH63" s="0"/>
       <c r="AMI63" s="0"/>
       <c r="AMJ63" s="0"/>
@@ -8759,9 +8766,9 @@
         <f aca="false">parameters!A79</f>
         <v>#subsection Geometry</v>
       </c>
-      <c r="B79" s="49"/>
-      <c r="C79" s="49"/>
-      <c r="D79" s="49"/>
+      <c r="B79" s="50"/>
+      <c r="C79" s="50"/>
+      <c r="D79" s="50"/>
       <c r="AMH79" s="0"/>
       <c r="AMI79" s="0"/>
       <c r="AMJ79" s="0"/>
@@ -8868,9 +8875,9 @@
         <f aca="false">parameters!A91</f>
         <v>#subsection Modeling</v>
       </c>
-      <c r="B91" s="49"/>
-      <c r="C91" s="49"/>
-      <c r="D91" s="49"/>
+      <c r="B91" s="50"/>
+      <c r="C91" s="50"/>
+      <c r="D91" s="50"/>
       <c r="AMH91" s="0"/>
       <c r="AMI91" s="0"/>
       <c r="AMJ91" s="0"/>
@@ -9136,7 +9143,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="22" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9154,7 +9161,7 @@
         <v># Legend: _</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9403,7 +9410,7 @@
         <f aca="false">parameters!A34</f>
         <v>Numerical Example</v>
       </c>
-      <c r="B34" s="49" t="n">
+      <c r="B34" s="50" t="n">
         <v>14</v>
       </c>
     </row>
@@ -9450,7 +9457,7 @@
         <f aca="false">parameters!A39</f>
         <v>Automatic Differentiation level</v>
       </c>
-      <c r="B39" s="56" t="n">
+      <c r="B39" s="57" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9518,7 +9525,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="73" t="str">
+      <c r="A48" s="74" t="str">
         <f aca="false">parameters!A48</f>
         <v>// plasticity parameters</v>
       </c>
@@ -9629,7 +9636,7 @@
       <c r="B62" s="0"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="73" t="str">
+      <c r="A63" s="74" t="str">
         <f aca="false">parameters!A63</f>
         <v>// damage parameters</v>
       </c>
@@ -10911,17 +10918,18 @@
   <dimension ref="A1:AMJ114"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q71" activeCellId="0" sqref="Q71"/>
+      <selection pane="topLeft" activeCell="J106" activeCellId="0" sqref="J106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="41.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="2" width="10.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="21.02"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="10" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="2" style="2" width="10.32"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="2" width="21.02"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="8" min="7" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="9" min="9" style="0" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.1"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="11" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="10.32"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
   </cols>
@@ -10946,7 +10954,7 @@
         <f aca="false">parameters!$A$2</f>
         <v>#export column marked by “x”</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>103</v>
       </c>
     </row>
@@ -11103,7 +11111,7 @@
         <v>100</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="K7" s="2" t="n">
         <v>15</v>
@@ -11154,7 +11162,7 @@
         <v>3</v>
       </c>
       <c r="J8" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="2" t="n">
         <v>0</v>
@@ -11212,7 +11220,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="J9" s="8" t="n">
+      <c r="J9" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -11278,7 +11286,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="J10" s="8" t="n">
+      <c r="J10" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -11337,7 +11345,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K11" s="2" t="n">
         <v>2</v>
@@ -11388,7 +11396,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K12" s="2" t="n">
         <v>0</v>
@@ -11796,7 +11804,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J22" s="2" t="n">
+      <c r="J22" s="25" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -12337,7 +12345,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="J35" s="8" t="n">
+      <c r="J35" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -12403,7 +12411,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J36" s="8" t="n">
+      <c r="J36" s="9" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12463,7 +12471,7 @@
         <v>1</v>
       </c>
       <c r="J37" s="10" t="n">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="K37" s="10" t="n">
         <v>0.1</v>
@@ -12514,7 +12522,7 @@
         <v>1E-006</v>
       </c>
       <c r="J38" s="11" t="n">
-        <v>1E-006</v>
+        <v>0.001</v>
       </c>
       <c r="K38" s="11" t="n">
         <v>1E-006</v>
@@ -12558,7 +12566,7 @@
         <v>1</v>
       </c>
       <c r="J39" s="28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K39" s="28" t="n">
         <v>1</v>
@@ -12691,7 +12699,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J44" s="0" t="n">
+      <c r="J44" s="16" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -13040,7 +13048,7 @@
         <v>400</v>
       </c>
       <c r="J52" s="20" t="n">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="K52" s="20" t="n">
         <v>-1000</v>
@@ -13176,10 +13184,6 @@
         <v>0</v>
       </c>
       <c r="I55" s="8" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J55" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -13305,9 +13309,6 @@
       <c r="I65" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="J65" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="M65" s="0" t="n">
         <v>0</v>
       </c>
@@ -13346,9 +13347,6 @@
       <c r="I66" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="J66" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="M66" s="0" t="n">
         <v>0</v>
       </c>
@@ -13387,9 +13385,6 @@
       <c r="I67" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="J67" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="M67" s="0" t="n">
         <v>0</v>
       </c>
@@ -13427,9 +13422,6 @@
       </c>
       <c r="I68" s="8" t="n">
         <v>0.5</v>
-      </c>
-      <c r="J68" s="0" t="n">
-        <v>0</v>
       </c>
       <c r="M68" s="0" t="n">
         <v>0</v>
@@ -13455,9 +13447,6 @@
       <c r="G69" s="8"/>
       <c r="H69" s="8"/>
       <c r="I69" s="8"/>
-      <c r="J69" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="M69" s="0" t="n">
         <v>0</v>
       </c>
@@ -13489,9 +13478,7 @@
       <c r="I70" s="10" t="n">
         <v>0.1</v>
       </c>
-      <c r="J70" s="20" t="n">
-        <v>1000000</v>
-      </c>
+      <c r="J70" s="20"/>
       <c r="K70" s="20" t="n">
         <v>1000000</v>
       </c>
@@ -13535,9 +13522,6 @@
       <c r="I71" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="J71" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="K71" s="0" t="n">
         <v>0</v>
       </c>
@@ -13581,9 +13565,6 @@
       <c r="I72" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="J72" s="0" t="n">
-        <v>100</v>
-      </c>
       <c r="K72" s="0" t="n">
         <v>100</v>
       </c>
@@ -13609,9 +13590,6 @@
       <c r="F73" s="27"/>
       <c r="G73" s="10"/>
       <c r="I73" s="2"/>
-      <c r="J73" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="K73" s="20" t="n">
         <v>1000</v>
       </c>
@@ -13631,9 +13609,6 @@
       <c r="F74" s="27"/>
       <c r="G74" s="10"/>
       <c r="I74" s="2"/>
-      <c r="J74" s="0" t="n">
-        <v>100</v>
-      </c>
       <c r="K74" s="20" t="n">
         <v>10000</v>
       </c>
@@ -14040,7 +14015,7 @@
         <v>11</v>
       </c>
       <c r="J88" s="2" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="K88" s="0" t="n">
         <v>20</v>
@@ -14162,7 +14137,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J98" s="8" t="n">
+      <c r="J98" s="9" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -14220,10 +14195,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="J99" s="8" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+      <c r="J99" s="9"/>
       <c r="M99" s="8" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -14278,10 +14250,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="J100" s="8" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+      <c r="J100" s="9"/>
       <c r="M100" s="8" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -14381,10 +14350,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="J102" s="8" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+      <c r="J102" s="9"/>
       <c r="M102" s="8" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -14439,10 +14405,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="J103" s="8" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+      <c r="J103" s="8"/>
       <c r="M103" s="8" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -14542,7 +14505,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="J105" s="8" t="n">
+      <c r="J105" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -14600,9 +14563,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J106" s="8" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J106" s="37" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="M106" s="8" t="n">
         <f aca="false">TRUE()</f>
@@ -14719,29 +14682,29 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="37" t="s">
+      <c r="A112" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="K112" s="38" t="s">
+      <c r="K112" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="L112" s="38" t="s">
+      <c r="L112" s="39" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="39" t="s">
+      <c r="A113" s="40" t="s">
         <v>121</v>
       </c>
-      <c r="K113" s="40" t="s">
+      <c r="K113" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="L113" s="40" t="s">
+      <c r="L113" s="41" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="39" t="s">
+      <c r="A114" s="40" t="s">
         <v>123</v>
       </c>
     </row>
@@ -14997,10 +14960,10 @@
       <c r="J8" s="23" t="n">
         <v>0</v>
       </c>
-      <c r="K8" s="41" t="n">
+      <c r="K8" s="42" t="n">
         <v>3</v>
       </c>
-      <c r="L8" s="41" t="n">
+      <c r="L8" s="42" t="n">
         <v>0</v>
       </c>
       <c r="M8" s="23" t="n">
@@ -15184,7 +15147,7 @@
       <c r="K13" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="L13" s="41" t="n">
+      <c r="L13" s="42" t="n">
         <v>2</v>
       </c>
       <c r="M13" s="23" t="n">
@@ -15845,7 +15808,7 @@
       <c r="I34" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="J34" s="42" t="n">
+      <c r="J34" s="43" t="n">
         <v>13</v>
       </c>
       <c r="K34" s="2" t="n">
@@ -15854,13 +15817,13 @@
       <c r="L34" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="M34" s="42" t="n">
-        <v>2</v>
-      </c>
-      <c r="N34" s="42" t="n">
+      <c r="M34" s="43" t="n">
+        <v>2</v>
+      </c>
+      <c r="N34" s="43" t="n">
         <v>13</v>
       </c>
-      <c r="O34" s="42" t="n">
+      <c r="O34" s="43" t="n">
         <v>13</v>
       </c>
     </row>
@@ -16231,15 +16194,15 @@
         <v>1</v>
       </c>
       <c r="F44" s="16"/>
-      <c r="G44" s="43" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H44" s="43" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I44" s="43" t="n">
+      <c r="G44" s="44" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H44" s="44" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I44" s="44" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -16291,7 +16254,7 @@
       <c r="H45" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="I45" s="44" t="n">
+      <c r="I45" s="45" t="n">
         <v>1</v>
       </c>
       <c r="J45" s="8" t="n">
@@ -16345,10 +16308,10 @@
       <c r="J46" s="31" t="n">
         <v>195000</v>
       </c>
-      <c r="K46" s="45" t="n">
+      <c r="K46" s="46" t="n">
         <v>63000</v>
       </c>
-      <c r="L46" s="45" t="n">
+      <c r="L46" s="46" t="n">
         <v>63000</v>
       </c>
       <c r="M46" s="31" t="n">
@@ -16375,10 +16338,10 @@
       <c r="D47" s="4" t="n">
         <v>0.340000016335238</v>
       </c>
-      <c r="E47" s="46" t="n">
+      <c r="E47" s="47" t="n">
         <v>0.2</v>
       </c>
-      <c r="F47" s="46" t="n">
+      <c r="F47" s="47" t="n">
         <v>0.340000016335238</v>
       </c>
       <c r="G47" s="8" t="n">
@@ -16390,22 +16353,22 @@
       <c r="I47" s="8" t="n">
         <v>0.499</v>
       </c>
-      <c r="J47" s="45" t="n">
+      <c r="J47" s="46" t="n">
         <v>0.3</v>
       </c>
-      <c r="K47" s="45" t="n">
+      <c r="K47" s="46" t="n">
         <v>0.34</v>
       </c>
-      <c r="L47" s="45" t="n">
+      <c r="L47" s="46" t="n">
         <v>0.34</v>
       </c>
-      <c r="M47" s="45" t="n">
+      <c r="M47" s="46" t="n">
         <v>0.3</v>
       </c>
-      <c r="N47" s="45" t="n">
+      <c r="N47" s="46" t="n">
         <v>0.3</v>
       </c>
-      <c r="O47" s="45" t="n">
+      <c r="O47" s="46" t="n">
         <v>0.3</v>
       </c>
     </row>
@@ -16508,7 +16471,7 @@
       <c r="G51" s="11" t="n">
         <v>10</v>
       </c>
-      <c r="H51" s="47" t="n">
+      <c r="H51" s="48" t="n">
         <v>40000</v>
       </c>
       <c r="I51" s="11" t="n">
@@ -16898,9 +16861,9 @@
       <c r="D63" s="18"/>
       <c r="E63" s="18"/>
       <c r="F63" s="18"/>
-      <c r="G63" s="48"/>
-      <c r="H63" s="48"/>
-      <c r="I63" s="48"/>
+      <c r="G63" s="49"/>
+      <c r="H63" s="49"/>
+      <c r="I63" s="49"/>
       <c r="J63" s="18"/>
       <c r="M63" s="18"/>
       <c r="N63" s="18"/>
@@ -17220,9 +17183,9 @@
       <c r="C79" s="6"/>
       <c r="D79" s="6"/>
       <c r="E79" s="6"/>
-      <c r="G79" s="49"/>
-      <c r="H79" s="49"/>
-      <c r="I79" s="49"/>
+      <c r="G79" s="50"/>
+      <c r="H79" s="50"/>
+      <c r="I79" s="50"/>
       <c r="J79" s="6"/>
       <c r="M79" s="6"/>
       <c r="N79" s="6"/>
@@ -17443,9 +17406,9 @@
       <c r="C91" s="6"/>
       <c r="D91" s="6"/>
       <c r="E91" s="6"/>
-      <c r="G91" s="49"/>
-      <c r="H91" s="49"/>
-      <c r="I91" s="49"/>
+      <c r="G91" s="50"/>
+      <c r="H91" s="50"/>
+      <c r="I91" s="50"/>
       <c r="J91" s="6"/>
       <c r="M91" s="6"/>
       <c r="N91" s="6"/>
@@ -18061,10 +18024,10 @@
       <c r="G106" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="H106" s="50" t="n">
+      <c r="H106" s="51" t="n">
         <v>3</v>
       </c>
-      <c r="I106" s="50" t="n">
+      <c r="I106" s="51" t="n">
         <v>2</v>
       </c>
       <c r="J106" s="8" t="n">
@@ -18462,7 +18425,7 @@
       <c r="F13" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="G13" s="51" t="n">
+      <c r="G13" s="52" t="n">
         <v>1</v>
       </c>
       <c r="H13" s="8" t="n">
@@ -18496,7 +18459,7 @@
       <c r="F14" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="G14" s="51" t="n">
+      <c r="G14" s="52" t="n">
         <v>3</v>
       </c>
       <c r="H14" s="8" t="n">
@@ -20646,8 +20609,8 @@
   </sheetPr>
   <dimension ref="A1:AA110"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z13" activeCellId="0" sqref="Z13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA4" activeCellId="0" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20671,7 +20634,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="14" width="13.66"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="23" min="23" style="14" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="14" width="13.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="26" style="14" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="26" min="26" style="14" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="13.1"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="28" style="14" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20698,13 +20663,14 @@
       <c r="X1" s="22"/>
       <c r="Y1" s="22"/>
       <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="str">
         <f aca="false">parameters!$A$2</f>
         <v>#export column marked by “x”</v>
       </c>
-      <c r="Z2" s="14" t="s">
+      <c r="AA2" s="0" t="s">
         <v>103</v>
       </c>
     </row>
@@ -20782,7 +20748,9 @@
       <c r="Z3" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="AA3" s="0"/>
+      <c r="AA3" s="0" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="str">
@@ -20812,8 +20780,8 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
     </row>
-    <row r="5" s="52" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="52" t="str">
+    <row r="5" s="53" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="53" t="str">
         <f aca="false">parameters!$A$5</f>
         <v>#subsection General</v>
       </c>
@@ -20833,6 +20801,7 @@
       <c r="X5" s="6"/>
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
+      <c r="AA5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="str">
@@ -20906,6 +20875,9 @@
       <c r="Z6" s="8" t="n">
         <v>0</v>
       </c>
+      <c r="AA6" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="str">
@@ -20979,6 +20951,9 @@
       <c r="Z7" s="8" t="n">
         <v>100</v>
       </c>
+      <c r="AA7" s="2" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="14" t="str">
@@ -21051,6 +21026,9 @@
       </c>
       <c r="Z8" s="8" t="n">
         <v>3</v>
+      </c>
+      <c r="AA8" s="2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21108,6 +21086,10 @@
       <c r="X9" s="8"/>
       <c r="Y9" s="8"/>
       <c r="Z9" s="8"/>
+      <c r="AA9" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="str">
@@ -21164,6 +21146,10 @@
       <c r="X10" s="8"/>
       <c r="Y10" s="8"/>
       <c r="Z10" s="8"/>
+      <c r="AA10" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="14" t="str">
@@ -21237,6 +21223,9 @@
       <c r="Z11" s="8" t="n">
         <v>0</v>
       </c>
+      <c r="AA11" s="2" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="str">
@@ -21310,6 +21299,9 @@
       <c r="Z12" s="8" t="n">
         <v>3</v>
       </c>
+      <c r="AA12" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="14" t="str">
@@ -21326,7 +21318,7 @@
       <c r="E13" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="F13" s="50" t="n">
+      <c r="F13" s="51" t="n">
         <v>2</v>
       </c>
       <c r="G13" s="8" t="n">
@@ -21374,13 +21366,16 @@
       <c r="W13" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="X13" s="53" t="n">
-        <v>2</v>
-      </c>
-      <c r="Y13" s="53" t="n">
+      <c r="X13" s="54" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y13" s="54" t="n">
         <v>2</v>
       </c>
       <c r="Z13" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA13" s="2" t="n">
         <v>2</v>
       </c>
     </row>
@@ -21423,9 +21418,10 @@
       <c r="U14" s="8"/>
       <c r="V14" s="8"/>
       <c r="W14" s="8"/>
-      <c r="X14" s="53"/>
-      <c r="Y14" s="53"/>
+      <c r="X14" s="54"/>
+      <c r="Y14" s="54"/>
       <c r="Z14" s="8"/>
+      <c r="AA14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="8"/>
@@ -21442,24 +21438,25 @@
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
-      <c r="N15" s="54"/>
-      <c r="P15" s="51" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="51" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="R15" s="54"/>
-      <c r="S15" s="54"/>
-      <c r="T15" s="54"/>
+      <c r="N15" s="55"/>
+      <c r="P15" s="52" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="52" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="R15" s="55"/>
+      <c r="S15" s="55"/>
+      <c r="T15" s="55"/>
       <c r="U15" s="9"/>
       <c r="V15" s="9"/>
       <c r="W15" s="9"/>
       <c r="X15" s="9"/>
       <c r="Y15" s="9"/>
       <c r="Z15" s="9"/>
+      <c r="AA15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="8"/>
@@ -21485,6 +21482,7 @@
       <c r="X16" s="9"/>
       <c r="Y16" s="9"/>
       <c r="Z16" s="9"/>
+      <c r="AA16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="14" t="str">
@@ -21558,13 +21556,16 @@
       <c r="Z17" s="8" t="n">
         <v>100</v>
       </c>
+      <c r="AA17" s="2" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="14" t="str">
         <f aca="false">parameters!A18</f>
         <v>Tolerance residual</v>
       </c>
-      <c r="B18" s="55" t="n">
+      <c r="B18" s="56" t="n">
         <v>1E-008</v>
       </c>
       <c r="C18" s="0"/>
@@ -21629,6 +21630,9 @@
         <v>1E-006</v>
       </c>
       <c r="Z18" s="11" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="AA18" s="10" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -21637,7 +21641,7 @@
         <f aca="false">parameters!A19</f>
         <v>NR window bottom</v>
       </c>
-      <c r="B19" s="55"/>
+      <c r="B19" s="56"/>
       <c r="C19" s="0"/>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
@@ -21690,13 +21694,16 @@
       <c r="Z19" s="24" t="n">
         <v>20</v>
       </c>
+      <c r="AA19" s="2" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="14" t="str">
         <f aca="false">parameters!A20</f>
         <v>NR window top</v>
       </c>
-      <c r="B20" s="55"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="0"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
@@ -21719,6 +21726,7 @@
       <c r="X20" s="11"/>
       <c r="Y20" s="11"/>
       <c r="Z20" s="11"/>
+      <c r="AA20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="14" t="str">
@@ -21791,6 +21799,9 @@
       </c>
       <c r="Z21" s="24" t="n">
         <v>100</v>
+      </c>
+      <c r="AA21" s="2" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21844,6 +21855,10 @@
       <c r="X22" s="9"/>
       <c r="Y22" s="9"/>
       <c r="Z22" s="9"/>
+      <c r="AA22" s="25" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="14" t="str">
@@ -21880,6 +21895,7 @@
       <c r="Z23" s="11" t="n">
         <v>1E-006</v>
       </c>
+      <c r="AA23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="14" t="str">
@@ -21912,6 +21928,7 @@
         <v>30</v>
       </c>
       <c r="Z24" s="8"/>
+      <c r="AA24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="14" t="str">
@@ -21977,6 +21994,9 @@
         <v>1</v>
       </c>
       <c r="Z25" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA25" s="2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -22026,6 +22046,7 @@
       <c r="X26" s="8"/>
       <c r="Y26" s="8"/>
       <c r="Z26" s="8"/>
+      <c r="AA26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="14" t="str">
@@ -22073,6 +22094,7 @@
       <c r="X27" s="8"/>
       <c r="Y27" s="8"/>
       <c r="Z27" s="8"/>
+      <c r="AA27" s="9"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="14" t="str">
@@ -22145,6 +22167,9 @@
       </c>
       <c r="Z28" s="8" t="n">
         <v>0.04</v>
+      </c>
+      <c r="AA28" s="2" t="n">
+        <v>0.004</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22174,6 +22199,7 @@
       <c r="X29" s="8"/>
       <c r="Y29" s="8"/>
       <c r="Z29" s="8"/>
+      <c r="AA29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="14" t="str">
@@ -22202,6 +22228,7 @@
       <c r="X30" s="8"/>
       <c r="Y30" s="8"/>
       <c r="Z30" s="8"/>
+      <c r="AA30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="14" t="str">
@@ -22252,6 +22279,7 @@
       <c r="X31" s="8"/>
       <c r="Y31" s="8"/>
       <c r="Z31" s="8"/>
+      <c r="AA31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="14" t="str">
@@ -22325,6 +22353,9 @@
       <c r="Z32" s="8" t="n">
         <v>2</v>
       </c>
+      <c r="AA32" s="8" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="14" t="str">
@@ -22398,6 +22429,9 @@
       <c r="Z33" s="8" t="n">
         <v>1</v>
       </c>
+      <c r="AA33" s="2" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="14" t="str">
@@ -22471,6 +22505,9 @@
       <c r="Z34" s="8" t="n">
         <v>1</v>
       </c>
+      <c r="AA34" s="2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="14" t="str">
@@ -22566,6 +22603,10 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="AA35" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="14" t="str">
@@ -22661,6 +22702,10 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="AA36" s="9" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="14" t="str">
@@ -22734,13 +22779,16 @@
       <c r="Z37" s="8" t="n">
         <v>0.3</v>
       </c>
+      <c r="AA37" s="10" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="14" t="str">
         <f aca="false">parameters!$A$38</f>
         <v>Min load increment</v>
       </c>
-      <c r="B38" s="55" t="n">
+      <c r="B38" s="56" t="n">
         <v>1E-006</v>
       </c>
       <c r="C38" s="0"/>
@@ -22807,12 +22855,15 @@
       <c r="Z38" s="11" t="n">
         <v>1E-006</v>
       </c>
+      <c r="AA38" s="11" t="n">
+        <v>0.001</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="55"/>
+      <c r="B39" s="56"/>
       <c r="C39" s="0"/>
       <c r="D39" s="11"/>
       <c r="E39" s="11"/>
@@ -22855,22 +22906,25 @@
       <c r="T39" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="U39" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="V39" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="W39" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="X39" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y39" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z39" s="56" t="n">
+      <c r="U39" s="57" t="n">
+        <v>1</v>
+      </c>
+      <c r="V39" s="57" t="n">
+        <v>1</v>
+      </c>
+      <c r="W39" s="57" t="n">
+        <v>1</v>
+      </c>
+      <c r="X39" s="57" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y39" s="57" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z39" s="57" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA39" s="28" t="n">
         <v>1</v>
       </c>
     </row>
@@ -22879,7 +22933,7 @@
         <f aca="false">parameters!$A$40</f>
         <v>#end</v>
       </c>
-      <c r="B40" s="55"/>
+      <c r="B40" s="56"/>
       <c r="C40" s="0"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -22904,7 +22958,7 @@
       <c r="Z40" s="2"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="55"/>
+      <c r="B41" s="56"/>
       <c r="C41" s="0"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -22929,11 +22983,11 @@
       <c r="Z41" s="2"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="52" t="str">
+      <c r="A42" s="53" t="str">
         <f aca="false">parameters!$A$42</f>
         <v>#subsection MaterialModel</v>
       </c>
-      <c r="B42" s="57"/>
+      <c r="B42" s="58"/>
       <c r="C42" s="7"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
@@ -22956,6 +23010,7 @@
       <c r="X42" s="6"/>
       <c r="Y42" s="6"/>
       <c r="Z42" s="6"/>
+      <c r="AA42" s="7"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="14" t="str">
@@ -23032,6 +23087,9 @@
       <c r="Z43" s="8" t="n">
         <v>8</v>
       </c>
+      <c r="AA43" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="14" t="str">
@@ -23063,11 +23121,11 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I44" s="43" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J44" s="43" t="n">
+      <c r="I44" s="44" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J44" s="44" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -23128,6 +23186,10 @@
         <v>1</v>
       </c>
       <c r="Z44" s="8" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="AA44" s="16" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -23207,6 +23269,9 @@
       <c r="Z45" s="8" t="n">
         <v>0</v>
       </c>
+      <c r="AA45" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="14" t="str">
@@ -23283,6 +23348,9 @@
       <c r="Z46" s="11" t="n">
         <v>18000</v>
       </c>
+      <c r="AA46" s="20" t="n">
+        <v>210000</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="14" t="str">
@@ -23359,13 +23427,16 @@
       <c r="Z47" s="8" t="n">
         <v>0.2</v>
       </c>
+      <c r="AA47" s="0" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="58" t="str">
+      <c r="A48" s="59" t="str">
         <f aca="false">parameters!$A$48</f>
         <v>// plasticity parameters</v>
       </c>
-      <c r="B48" s="59"/>
+      <c r="B48" s="60"/>
       <c r="C48" s="19"/>
       <c r="D48" s="18"/>
       <c r="E48" s="18"/>
@@ -23389,6 +23460,7 @@
       <c r="X48" s="18"/>
       <c r="Y48" s="18"/>
       <c r="Z48" s="18"/>
+      <c r="AA48" s="19"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="14" t="str">
@@ -23423,28 +23495,28 @@
       <c r="K49" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="L49" s="51" t="n">
+      <c r="L49" s="52" t="n">
         <v>3</v>
       </c>
-      <c r="M49" s="51" t="n">
+      <c r="M49" s="52" t="n">
         <v>3</v>
       </c>
-      <c r="N49" s="51" t="n">
-        <v>0</v>
-      </c>
-      <c r="P49" s="51" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q49" s="51" t="n">
-        <v>1</v>
-      </c>
-      <c r="R49" s="51" t="n">
-        <v>0</v>
-      </c>
-      <c r="S49" s="51" t="n">
-        <v>1</v>
-      </c>
-      <c r="T49" s="51" t="n">
+      <c r="N49" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="P49" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="R49" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="S49" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="T49" s="52" t="n">
         <v>2</v>
       </c>
       <c r="U49" s="8" t="n">
@@ -23464,6 +23536,9 @@
       </c>
       <c r="Z49" s="8" t="n">
         <v>3</v>
+      </c>
+      <c r="AA49" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23572,13 +23647,16 @@
       <c r="Z51" s="11" t="n">
         <v>40</v>
       </c>
+      <c r="AA51" s="0" t="n">
+        <v>400</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="14" t="str">
         <f aca="false">parameters!$A$52</f>
         <v>Hardening modulus K</v>
       </c>
-      <c r="B52" s="55" t="n">
+      <c r="B52" s="56" t="n">
         <v>100</v>
       </c>
       <c r="C52" s="0"/>
@@ -23642,11 +23720,14 @@
       <c r="X52" s="11" t="n">
         <v>100</v>
       </c>
-      <c r="Y52" s="60" t="n">
+      <c r="Y52" s="61" t="n">
         <v>0</v>
       </c>
       <c r="Z52" s="11" t="n">
         <v>10</v>
+      </c>
+      <c r="AA52" s="20" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23654,7 +23735,7 @@
         <f aca="false">parameters!$A$53</f>
         <v>Hardening modulus of exp</v>
       </c>
-      <c r="B53" s="61" t="n">
+      <c r="B53" s="62" t="n">
         <v>12</v>
       </c>
       <c r="C53" s="0"/>
@@ -23708,7 +23789,7 @@
       <c r="X53" s="21" t="n">
         <v>16.93</v>
       </c>
-      <c r="Y53" s="62" t="n">
+      <c r="Y53" s="63" t="n">
         <v>5</v>
       </c>
       <c r="Z53" s="21" t="n">
@@ -23817,11 +23898,11 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I55" s="50" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J55" s="50" t="n">
+      <c r="I55" s="51" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J55" s="51" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24190,34 +24271,35 @@
       <c r="Z62" s="8"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="58" t="str">
+      <c r="A63" s="59" t="str">
         <f aca="false">parameters!$A$63</f>
         <v>// damage parameters</v>
       </c>
-      <c r="B63" s="59"/>
+      <c r="B63" s="60"/>
       <c r="C63" s="19"/>
-      <c r="D63" s="48"/>
-      <c r="E63" s="48"/>
-      <c r="F63" s="48"/>
-      <c r="G63" s="48"/>
-      <c r="H63" s="48"/>
-      <c r="I63" s="48"/>
-      <c r="J63" s="48"/>
-      <c r="K63" s="48"/>
-      <c r="L63" s="48"/>
-      <c r="M63" s="48"/>
-      <c r="N63" s="48"/>
-      <c r="P63" s="48"/>
-      <c r="Q63" s="48"/>
-      <c r="R63" s="48"/>
-      <c r="S63" s="48"/>
-      <c r="T63" s="48"/>
-      <c r="U63" s="48"/>
-      <c r="V63" s="48"/>
-      <c r="W63" s="48"/>
-      <c r="X63" s="48"/>
-      <c r="Y63" s="48"/>
-      <c r="Z63" s="48"/>
+      <c r="D63" s="49"/>
+      <c r="E63" s="49"/>
+      <c r="F63" s="49"/>
+      <c r="G63" s="49"/>
+      <c r="H63" s="49"/>
+      <c r="I63" s="49"/>
+      <c r="J63" s="49"/>
+      <c r="K63" s="49"/>
+      <c r="L63" s="49"/>
+      <c r="M63" s="49"/>
+      <c r="N63" s="49"/>
+      <c r="P63" s="49"/>
+      <c r="Q63" s="49"/>
+      <c r="R63" s="49"/>
+      <c r="S63" s="49"/>
+      <c r="T63" s="49"/>
+      <c r="U63" s="49"/>
+      <c r="V63" s="49"/>
+      <c r="W63" s="49"/>
+      <c r="X63" s="49"/>
+      <c r="Y63" s="49"/>
+      <c r="Z63" s="49"/>
+      <c r="AA63" s="19"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="14" t="str">
@@ -24339,7 +24421,7 @@
         <v>Exp. rate param. eta_2</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C66" s="0"/>
       <c r="D66" s="2" t="n">
@@ -24443,31 +24525,31 @@
       <c r="K67" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="L67" s="63" t="n">
+      <c r="L67" s="64" t="n">
         <v>0.25</v>
       </c>
-      <c r="M67" s="63" t="n">
+      <c r="M67" s="64" t="n">
         <v>0.25</v>
       </c>
-      <c r="N67" s="63" t="n">
+      <c r="N67" s="64" t="n">
         <v>0.05</v>
       </c>
-      <c r="O67" s="63" t="n">
+      <c r="O67" s="64" t="n">
         <v>0.1</v>
       </c>
-      <c r="P67" s="63" t="n">
+      <c r="P67" s="64" t="n">
         <v>10</v>
       </c>
-      <c r="Q67" s="63" t="n">
+      <c r="Q67" s="64" t="n">
         <v>10000</v>
       </c>
-      <c r="R67" s="63" t="n">
+      <c r="R67" s="64" t="n">
         <v>1000000</v>
       </c>
-      <c r="S67" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="T67" s="63" t="n">
+      <c r="S67" s="64" t="n">
+        <v>1</v>
+      </c>
+      <c r="T67" s="64" t="n">
         <v>0</v>
       </c>
       <c r="U67" s="10"/>
@@ -24493,7 +24575,7 @@
         <v>Exp. rate param. eta_4</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C68" s="0"/>
       <c r="D68" s="2" t="n">
@@ -24608,7 +24690,7 @@
         <v>q_min</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C70" s="0"/>
       <c r="D70" s="8" t="n">
@@ -24672,12 +24754,13 @@
       <c r="X70" s="11" t="n">
         <v>0.4</v>
       </c>
-      <c r="Y70" s="64" t="n">
+      <c r="Y70" s="65" t="n">
         <v>0.4</v>
       </c>
       <c r="Z70" s="8" t="n">
         <v>0.4</v>
       </c>
+      <c r="AA70" s="20"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="14" t="str">
@@ -24724,7 +24807,7 @@
       <c r="O71" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="P71" s="64" t="n">
+      <c r="P71" s="65" t="n">
         <v>200</v>
       </c>
       <c r="Q71" s="11" t="n">
@@ -24899,7 +24982,7 @@
       <c r="O74" s="11"/>
       <c r="P74" s="11"/>
       <c r="Q74" s="11"/>
-      <c r="R74" s="65" t="n">
+      <c r="R74" s="66" t="n">
         <v>10000</v>
       </c>
       <c r="S74" s="11" t="n">
@@ -24919,7 +25002,7 @@
       <c r="Y74" s="11" t="n">
         <v>10000</v>
       </c>
-      <c r="Z74" s="66" t="n">
+      <c r="Z74" s="67" t="n">
         <v>100000</v>
       </c>
     </row>
@@ -25053,33 +25136,33 @@
       <c r="Z78" s="8"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="52" t="str">
+      <c r="A79" s="53" t="str">
         <f aca="false">parameters!$A$79</f>
         <v>#subsection Geometry</v>
       </c>
-      <c r="B79" s="57"/>
+      <c r="B79" s="58"/>
       <c r="C79" s="7"/>
-      <c r="D79" s="49"/>
-      <c r="E79" s="49"/>
-      <c r="F79" s="49"/>
-      <c r="G79" s="49"/>
-      <c r="H79" s="49"/>
-      <c r="I79" s="49"/>
-      <c r="K79" s="49"/>
-      <c r="L79" s="49"/>
-      <c r="M79" s="49"/>
-      <c r="N79" s="49"/>
-      <c r="P79" s="49"/>
-      <c r="Q79" s="49"/>
-      <c r="R79" s="49"/>
-      <c r="S79" s="49"/>
-      <c r="T79" s="49"/>
-      <c r="U79" s="49"/>
-      <c r="V79" s="49"/>
-      <c r="W79" s="49"/>
-      <c r="X79" s="49"/>
-      <c r="Y79" s="49"/>
-      <c r="Z79" s="49"/>
+      <c r="D79" s="50"/>
+      <c r="E79" s="50"/>
+      <c r="F79" s="50"/>
+      <c r="G79" s="50"/>
+      <c r="H79" s="50"/>
+      <c r="I79" s="50"/>
+      <c r="K79" s="50"/>
+      <c r="L79" s="50"/>
+      <c r="M79" s="50"/>
+      <c r="N79" s="50"/>
+      <c r="P79" s="50"/>
+      <c r="Q79" s="50"/>
+      <c r="R79" s="50"/>
+      <c r="S79" s="50"/>
+      <c r="T79" s="50"/>
+      <c r="U79" s="50"/>
+      <c r="V79" s="50"/>
+      <c r="W79" s="50"/>
+      <c r="X79" s="50"/>
+      <c r="Y79" s="50"/>
+      <c r="Z79" s="50"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="14" t="str">
@@ -25153,6 +25236,7 @@
       <c r="Z80" s="8" t="n">
         <v>100</v>
       </c>
+      <c r="AA80" s="7"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="14" t="str">
@@ -25226,6 +25310,9 @@
       <c r="Z81" s="8" t="n">
         <v>50</v>
       </c>
+      <c r="AA81" s="2" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="14" t="str">
@@ -25297,6 +25384,9 @@
       <c r="Z82" s="8" t="n">
         <v>20</v>
       </c>
+      <c r="AA82" s="2" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="14" t="str">
@@ -25308,7 +25398,7 @@
       </c>
       <c r="C83" s="0"/>
       <c r="D83" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E83" s="8" t="n">
         <v>1</v>
@@ -25368,6 +25458,7 @@
       <c r="Z83" s="8" t="n">
         <v>1</v>
       </c>
+      <c r="AA83" s="2"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="14" t="str">
@@ -25438,6 +25529,9 @@
       <c r="Y84" s="8"/>
       <c r="Z84" s="8" t="n">
         <v>1</v>
+      </c>
+      <c r="AA84" s="2" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25490,6 +25584,9 @@
       <c r="Z85" s="8" t="n">
         <v>8.98</v>
       </c>
+      <c r="AA85" s="2" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="14" t="str">
@@ -25560,6 +25657,9 @@
       <c r="Y86" s="8"/>
       <c r="Z86" s="8" t="n">
         <v>3</v>
+      </c>
+      <c r="AA86" s="2" t="n">
+        <v>1.4</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25612,6 +25712,7 @@
       <c r="Z87" s="8" t="n">
         <v>8</v>
       </c>
+      <c r="AA87" s="2"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="14" t="s">
@@ -25659,6 +25760,9 @@
       <c r="X88" s="8"/>
       <c r="Y88" s="8"/>
       <c r="Z88" s="8"/>
+      <c r="AA88" s="2" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="14" t="str">
@@ -25713,33 +25817,33 @@
       <c r="Z90" s="8"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="52" t="str">
+      <c r="A91" s="53" t="str">
         <f aca="false">parameters!$A$91</f>
         <v>#subsection Modeling</v>
       </c>
-      <c r="B91" s="57"/>
+      <c r="B91" s="58"/>
       <c r="C91" s="7"/>
-      <c r="D91" s="49"/>
-      <c r="E91" s="49"/>
-      <c r="F91" s="49"/>
-      <c r="G91" s="49"/>
-      <c r="H91" s="49"/>
-      <c r="I91" s="49"/>
-      <c r="K91" s="49"/>
-      <c r="L91" s="49"/>
-      <c r="M91" s="49"/>
-      <c r="N91" s="49"/>
-      <c r="P91" s="49"/>
-      <c r="Q91" s="49"/>
-      <c r="R91" s="49"/>
-      <c r="S91" s="49"/>
-      <c r="T91" s="49"/>
-      <c r="U91" s="49"/>
-      <c r="V91" s="49"/>
-      <c r="W91" s="49"/>
-      <c r="X91" s="49"/>
-      <c r="Y91" s="49"/>
-      <c r="Z91" s="49"/>
+      <c r="D91" s="50"/>
+      <c r="E91" s="50"/>
+      <c r="F91" s="50"/>
+      <c r="G91" s="50"/>
+      <c r="H91" s="50"/>
+      <c r="I91" s="50"/>
+      <c r="K91" s="50"/>
+      <c r="L91" s="50"/>
+      <c r="M91" s="50"/>
+      <c r="N91" s="50"/>
+      <c r="P91" s="50"/>
+      <c r="Q91" s="50"/>
+      <c r="R91" s="50"/>
+      <c r="S91" s="50"/>
+      <c r="T91" s="50"/>
+      <c r="U91" s="50"/>
+      <c r="V91" s="50"/>
+      <c r="W91" s="50"/>
+      <c r="X91" s="50"/>
+      <c r="Y91" s="50"/>
+      <c r="Z91" s="50"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="14" t="str">
@@ -25813,6 +25917,7 @@
       <c r="Z92" s="8" t="n">
         <v>1</v>
       </c>
+      <c r="AA92" s="7"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="14" t="str">
@@ -26250,6 +26355,10 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="AA98" s="9" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="14" t="str">
@@ -26345,6 +26454,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="AA99" s="9"/>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="14" t="str">
@@ -26418,6 +26528,7 @@
       <c r="Z100" s="8" t="n">
         <v>2</v>
       </c>
+      <c r="AA100" s="9"/>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="14" t="str">
@@ -26513,6 +26624,9 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="AA101" s="8" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="14" t="str">
@@ -26608,6 +26722,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="AA102" s="9"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="14" t="str">
@@ -26681,6 +26796,7 @@
       <c r="Z103" s="8" t="n">
         <v>0</v>
       </c>
+      <c r="AA103" s="8"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="14" t="str">
@@ -26776,6 +26892,9 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="AA104" s="8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="14" t="str">
@@ -26871,6 +26990,10 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="AA105" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="14" t="str">
@@ -26943,6 +27066,10 @@
       </c>
       <c r="Z106" s="8" t="n">
         <v>2</v>
+      </c>
+      <c r="AA106" s="37" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26967,6 +27094,9 @@
       <c r="X107" s="8"/>
       <c r="Y107" s="8"/>
       <c r="Z107" s="8"/>
+      <c r="AA107" s="8" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="14" t="s">
@@ -26989,6 +27119,7 @@
       <c r="X108" s="8"/>
       <c r="Y108" s="8"/>
       <c r="Z108" s="8"/>
+      <c r="AA108" s="8"/>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="14" t="str">
@@ -27038,7 +27169,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
@@ -27062,16 +27193,16 @@
         <v># Legend: _</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27091,8 +27222,8 @@
       <c r="K4" s="0"/>
       <c r="L4" s="0"/>
     </row>
-    <row r="5" s="52" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="52" t="str">
+    <row r="5" s="53" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="53" t="str">
         <f aca="false">parameters!$A$5</f>
         <v>#subsection General</v>
       </c>
@@ -27222,7 +27353,7 @@
         <f aca="false">parameters!A13</f>
         <v>Poly degree</v>
       </c>
-      <c r="B13" s="50" t="n">
+      <c r="B13" s="51" t="n">
         <v>1</v>
       </c>
       <c r="C13" s="8" t="n">
@@ -27643,7 +27774,7 @@
       <c r="E41" s="2"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="52" t="str">
+      <c r="A42" s="53" t="str">
         <f aca="false">parameters!$A$42</f>
         <v>#subsection MaterialModel</v>
       </c>
@@ -27679,15 +27810,15 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C44" s="67" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D44" s="67" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E44" s="67" t="n">
+      <c r="C44" s="68" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D44" s="68" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E44" s="68" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -27747,7 +27878,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="58" t="str">
+      <c r="A48" s="59" t="str">
         <f aca="false">parameters!$A$48</f>
         <v>// plasticity parameters</v>
       </c>
@@ -27861,15 +27992,15 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C55" s="68" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D55" s="68" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E55" s="68" t="n">
+      <c r="C55" s="69" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D55" s="69" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E55" s="69" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -28005,14 +28136,14 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="58" t="str">
+      <c r="A63" s="59" t="str">
         <f aca="false">parameters!$A$63</f>
         <v>// damage parameters</v>
       </c>
-      <c r="B63" s="48"/>
-      <c r="C63" s="48"/>
-      <c r="D63" s="48"/>
-      <c r="E63" s="48"/>
+      <c r="B63" s="49"/>
+      <c r="C63" s="49"/>
+      <c r="D63" s="49"/>
+      <c r="E63" s="49"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="14" t="str">
@@ -28214,14 +28345,14 @@
       <c r="E78" s="8"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="52" t="str">
+      <c r="A79" s="53" t="str">
         <f aca="false">parameters!$A$79</f>
         <v>#subsection Geometry</v>
       </c>
-      <c r="B79" s="49"/>
-      <c r="C79" s="49"/>
-      <c r="D79" s="49"/>
-      <c r="E79" s="49"/>
+      <c r="B79" s="50"/>
+      <c r="C79" s="50"/>
+      <c r="D79" s="50"/>
+      <c r="E79" s="50"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="14" t="str">
@@ -28246,7 +28377,7 @@
         <f aca="false">parameters!$A$81</f>
         <v>Hole radius</v>
       </c>
-      <c r="B81" s="69" t="n">
+      <c r="B81" s="70" t="n">
         <v>25</v>
       </c>
       <c r="C81" s="8" t="n">
@@ -28359,7 +28490,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="14" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B88" s="8"/>
       <c r="C88" s="8"/>
@@ -28383,14 +28514,14 @@
       <c r="E90" s="8"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="52" t="str">
+      <c r="A91" s="53" t="str">
         <f aca="false">parameters!$A$91</f>
         <v>#subsection Modeling</v>
       </c>
-      <c r="B91" s="49"/>
-      <c r="C91" s="49"/>
-      <c r="D91" s="49"/>
-      <c r="E91" s="49"/>
+      <c r="B91" s="50"/>
+      <c r="C91" s="50"/>
+      <c r="D91" s="50"/>
+      <c r="E91" s="50"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="14" t="str">
@@ -28694,8 +28825,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ110"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U46" activeCellId="0" sqref="U46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -28721,11 +28852,11 @@
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
       <c r="D1" s="22" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E1" s="22"/>
       <c r="F1" s="22" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G1" s="22"/>
       <c r="H1" s="22"/>
@@ -28752,53 +28883,53 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="46" t="s">
-        <v>178</v>
+      <c r="A3" s="47" t="s">
+        <v>179</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E3" s="46" t="s">
         <v>182</v>
       </c>
+      <c r="E3" s="47" t="s">
+        <v>183</v>
+      </c>
       <c r="F3" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="I3" s="46" t="s">
         <v>186</v>
       </c>
+      <c r="I3" s="47" t="s">
+        <v>187</v>
+      </c>
       <c r="J3" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="K3" s="46" t="s">
         <v>188</v>
       </c>
+      <c r="K3" s="47" t="s">
+        <v>189</v>
+      </c>
       <c r="L3" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29097,13 +29228,13 @@
       <c r="F12" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="G12" s="70" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="70" t="n">
+      <c r="G12" s="71" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="71" t="n">
         <v>10</v>
       </c>
-      <c r="I12" s="70" t="n">
+      <c r="I12" s="71" t="n">
         <v>4</v>
       </c>
       <c r="J12" s="8" t="n">
@@ -29115,7 +29246,7 @@
       <c r="L12" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="M12" s="70" t="n">
+      <c r="M12" s="71" t="n">
         <v>6</v>
       </c>
       <c r="N12" s="8" t="n">
@@ -29198,7 +29329,7 @@
       <c r="G14" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="H14" s="69" t="n">
+      <c r="H14" s="70" t="n">
         <v>2</v>
       </c>
       <c r="I14" s="8" t="n">
@@ -29213,7 +29344,7 @@
       <c r="L14" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="M14" s="69" t="n">
+      <c r="M14" s="70" t="n">
         <v>0</v>
       </c>
       <c r="N14" s="8" t="n">
@@ -30084,7 +30215,8 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="P36" s="9" t="b">
+      <c r="P36" s="9" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
@@ -30172,7 +30304,7 @@
       <c r="J38" s="11" t="n">
         <v>1E-006</v>
       </c>
-      <c r="K38" s="65" t="n">
+      <c r="K38" s="66" t="n">
         <v>0.02</v>
       </c>
       <c r="L38" s="11" t="n">
@@ -30340,31 +30472,31 @@
         <f aca="false">parameters!A44</f>
         <v>Use finite strains</v>
       </c>
-      <c r="B44" s="43" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C44" s="71" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D44" s="43" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E44" s="43" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F44" s="43" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G44" s="43" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H44" s="43" t="n">
+      <c r="B44" s="44" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C44" s="72" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D44" s="44" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E44" s="44" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F44" s="44" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G44" s="44" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H44" s="44" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -30372,31 +30504,31 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J44" s="43" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K44" s="43" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="L44" s="67" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M44" s="67" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="N44" s="67" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="O44" s="67" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="P44" s="67" t="n">
+      <c r="J44" s="44" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K44" s="44" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="L44" s="68" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="M44" s="68" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N44" s="68" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O44" s="68" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="P44" s="68" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -30409,7 +30541,7 @@
       <c r="B45" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="C45" s="51" t="n">
+      <c r="C45" s="52" t="n">
         <v>1</v>
       </c>
       <c r="D45" s="8" t="n">
@@ -30490,14 +30622,14 @@
       <c r="L46" s="11" t="n">
         <v>206900.647427708</v>
       </c>
-      <c r="M46" s="72" t="n">
+      <c r="M46" s="73" t="n">
         <v>199993.599916801</v>
       </c>
-      <c r="N46" s="72" t="n">
+      <c r="N46" s="73" t="n">
         <f aca="false">1000.00986663708</f>
         <v>1000.00986663708</v>
       </c>
-      <c r="O46" s="72" t="n">
+      <c r="O46" s="73" t="n">
         <f aca="false">1000.00986663708</f>
         <v>1000.00986663708</v>
       </c>
@@ -30557,7 +30689,7 @@
       </c>
     </row>
     <row r="48" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="73" t="str">
+      <c r="A48" s="74" t="str">
         <f aca="false">parameters!A48</f>
         <v>// plasticity parameters</v>
       </c>
@@ -30968,19 +31100,19 @@
       <c r="P62" s="8"/>
     </row>
     <row r="63" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="73" t="str">
+      <c r="A63" s="74" t="str">
         <f aca="false">parameters!A63</f>
         <v>// damage parameters</v>
       </c>
-      <c r="B63" s="48"/>
+      <c r="B63" s="49"/>
       <c r="C63" s="18"/>
-      <c r="D63" s="48"/>
-      <c r="E63" s="48"/>
-      <c r="F63" s="48"/>
-      <c r="G63" s="48"/>
-      <c r="J63" s="48"/>
-      <c r="L63" s="48"/>
-      <c r="P63" s="48"/>
+      <c r="D63" s="49"/>
+      <c r="E63" s="49"/>
+      <c r="F63" s="49"/>
+      <c r="G63" s="49"/>
+      <c r="J63" s="49"/>
+      <c r="L63" s="49"/>
+      <c r="P63" s="49"/>
       <c r="AMH63" s="0"/>
       <c r="AMI63" s="0"/>
       <c r="AMJ63" s="0"/>
@@ -31196,7 +31328,7 @@
       <c r="H74" s="20" t="n">
         <v>100000</v>
       </c>
-      <c r="J74" s="65" t="n">
+      <c r="J74" s="66" t="n">
         <v>10000</v>
       </c>
       <c r="K74" s="35"/>
@@ -31267,15 +31399,15 @@
         <f aca="false">parameters!A79</f>
         <v>#subsection Geometry</v>
       </c>
-      <c r="B79" s="49"/>
+      <c r="B79" s="50"/>
       <c r="C79" s="6"/>
-      <c r="D79" s="49"/>
-      <c r="E79" s="49"/>
-      <c r="F79" s="49"/>
-      <c r="G79" s="49"/>
-      <c r="J79" s="49"/>
-      <c r="L79" s="49"/>
-      <c r="P79" s="49"/>
+      <c r="D79" s="50"/>
+      <c r="E79" s="50"/>
+      <c r="F79" s="50"/>
+      <c r="G79" s="50"/>
+      <c r="J79" s="50"/>
+      <c r="L79" s="50"/>
+      <c r="P79" s="50"/>
       <c r="AMH79" s="0"/>
       <c r="AMI79" s="0"/>
       <c r="AMJ79" s="0"/>
@@ -31484,7 +31616,7 @@
       <c r="E85" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="F85" s="53" t="n">
+      <c r="F85" s="54" t="n">
         <f aca="false">F80</f>
         <v>53.334</v>
       </c>
@@ -31503,7 +31635,7 @@
       <c r="K85" s="8" t="n">
         <v>8.98</v>
       </c>
-      <c r="L85" s="53" t="n">
+      <c r="L85" s="54" t="n">
         <f aca="false">L80</f>
         <v>53.334</v>
       </c>
@@ -31516,7 +31648,7 @@
       <c r="O85" s="0" t="n">
         <v>1.5</v>
       </c>
-      <c r="P85" s="53" t="n">
+      <c r="P85" s="54" t="n">
         <f aca="false">P80</f>
         <v>53.34</v>
       </c>
@@ -31579,7 +31711,7 @@
       <c r="F88" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="G88" s="70" t="n">
+      <c r="G88" s="71" t="n">
         <v>2</v>
       </c>
       <c r="J88" s="8"/>
@@ -31628,15 +31760,15 @@
         <f aca="false">parameters!A91</f>
         <v>#subsection Modeling</v>
       </c>
-      <c r="B91" s="49"/>
+      <c r="B91" s="50"/>
       <c r="C91" s="6"/>
-      <c r="D91" s="49"/>
-      <c r="E91" s="49"/>
-      <c r="F91" s="49"/>
-      <c r="G91" s="49"/>
-      <c r="J91" s="49"/>
-      <c r="L91" s="49"/>
-      <c r="P91" s="49"/>
+      <c r="D91" s="50"/>
+      <c r="E91" s="50"/>
+      <c r="F91" s="50"/>
+      <c r="G91" s="50"/>
+      <c r="J91" s="50"/>
+      <c r="L91" s="50"/>
+      <c r="P91" s="50"/>
       <c r="AMH91" s="0"/>
       <c r="AMI91" s="0"/>
       <c r="AMJ91" s="0"/>
@@ -32370,7 +32502,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="22" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
@@ -32395,26 +32527,26 @@
         <v># Legend: _</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E3" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
+      <c r="E3" s="47" t="s">
+        <v>198</v>
+      </c>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="str">
@@ -32640,14 +32772,14 @@
       <c r="F13" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="G13" s="74" t="n">
-        <v>2</v>
-      </c>
-      <c r="H13" s="74" t="n">
+      <c r="G13" s="75" t="n">
+        <v>2</v>
+      </c>
+      <c r="H13" s="75" t="n">
         <v>2</v>
       </c>
       <c r="J13" s="8"/>
-      <c r="M13" s="75"/>
+      <c r="M13" s="76"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="str">
@@ -32692,7 +32824,7 @@
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
-      <c r="J15" s="76"/>
+      <c r="J15" s="77"/>
       <c r="M15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32971,7 +33103,7 @@
         <f aca="false">parameters!A28</f>
         <v>Initial increment</v>
       </c>
-      <c r="B28" s="77" t="n">
+      <c r="B28" s="78" t="n">
         <v>0.05</v>
       </c>
       <c r="C28" s="8" t="n">
@@ -33159,15 +33291,15 @@
         <f aca="false">parameters!A36</f>
         <v>GG-Mode</v>
       </c>
-      <c r="B36" s="78" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C36" s="78" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D36" s="78" t="n">
+      <c r="B36" s="79" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C36" s="79" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D36" s="79" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -33332,15 +33464,15 @@
         <f aca="false">parameters!A44</f>
         <v>Use finite strains</v>
       </c>
-      <c r="B44" s="43" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C44" s="43" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D44" s="43" t="n">
+      <c r="B44" s="44" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C44" s="44" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D44" s="44" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -33443,7 +33575,7 @@
       </c>
     </row>
     <row r="48" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="73" t="str">
+      <c r="A48" s="74" t="str">
         <f aca="false">parameters!A48</f>
         <v>// plasticity parameters</v>
       </c>
@@ -33742,13 +33874,13 @@
       </c>
     </row>
     <row r="63" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="73" t="str">
+      <c r="A63" s="74" t="str">
         <f aca="false">parameters!A63</f>
         <v>// damage parameters</v>
       </c>
-      <c r="B63" s="48"/>
-      <c r="C63" s="48"/>
-      <c r="D63" s="48"/>
+      <c r="B63" s="49"/>
+      <c r="C63" s="49"/>
+      <c r="D63" s="49"/>
       <c r="AMH63" s="0"/>
       <c r="AMI63" s="0"/>
       <c r="AMJ63" s="0"/>
@@ -33978,9 +34110,9 @@
         <f aca="false">parameters!A79</f>
         <v>#subsection Geometry</v>
       </c>
-      <c r="B79" s="49"/>
-      <c r="C79" s="49"/>
-      <c r="D79" s="49"/>
+      <c r="B79" s="50"/>
+      <c r="C79" s="50"/>
+      <c r="D79" s="50"/>
       <c r="AMH79" s="0"/>
       <c r="AMI79" s="0"/>
       <c r="AMJ79" s="0"/>
@@ -34195,9 +34327,9 @@
         <f aca="false">parameters!A91</f>
         <v>#subsection Modeling</v>
       </c>
-      <c r="B91" s="49"/>
-      <c r="C91" s="49"/>
-      <c r="D91" s="49"/>
+      <c r="B91" s="50"/>
+      <c r="C91" s="50"/>
+      <c r="D91" s="50"/>
       <c r="AMH91" s="0"/>
       <c r="AMI91" s="0"/>
       <c r="AMJ91" s="0"/>

</xml_diff>

<commit_message>
BUGfix: rows for QPlate-AMR were misaligned
</commit_message>
<xml_diff>
--- a/parameter_manager.xlsx
+++ b/parameter_manager.xlsx
@@ -1370,9 +1370,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>95040</xdr:colOff>
+      <xdr:colOff>94680</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>122400</xdr:rowOff>
+      <xdr:rowOff>122040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1382,7 +1382,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1000800" y="2806920"/>
-          <a:ext cx="5596560" cy="2679840"/>
+          <a:ext cx="5596200" cy="2679480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1481,9 +1481,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>146880</xdr:colOff>
+      <xdr:colOff>146520</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:rowOff>2520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1493,7 +1493,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1052640" y="693360"/>
-          <a:ext cx="5596560" cy="772560"/>
+          <a:ext cx="5596200" cy="772200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1544,9 +1544,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>136440</xdr:colOff>
+      <xdr:colOff>136080</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>46080</xdr:rowOff>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1556,7 +1556,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1042200" y="1711800"/>
-          <a:ext cx="5596560" cy="772560"/>
+          <a:ext cx="5596200" cy="772200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1607,9 +1607,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>84240</xdr:colOff>
+      <xdr:colOff>83880</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>143640</xdr:rowOff>
+      <xdr:rowOff>143280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1619,7 +1619,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="990000" y="5710680"/>
-          <a:ext cx="5596560" cy="772560"/>
+          <a:ext cx="5596200" cy="772200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10917,7 +10917,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J106" activeCellId="0" sqref="J106"/>
     </sheetView>
   </sheetViews>
@@ -20610,7 +20610,7 @@
   <dimension ref="A1:AA110"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA4" activeCellId="0" sqref="AA4"/>
+      <selection pane="topLeft" activeCell="AC79" activeCellId="0" sqref="AC79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25163,6 +25163,7 @@
       <c r="X79" s="50"/>
       <c r="Y79" s="50"/>
       <c r="Z79" s="50"/>
+      <c r="AA79" s="7"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="14" t="str">
@@ -25236,7 +25237,9 @@
       <c r="Z80" s="8" t="n">
         <v>100</v>
       </c>
-      <c r="AA80" s="7"/>
+      <c r="AA80" s="2" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="14" t="str">
@@ -25311,7 +25314,7 @@
         <v>50</v>
       </c>
       <c r="AA81" s="2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25384,9 +25387,7 @@
       <c r="Z82" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="AA82" s="2" t="n">
-        <v>2</v>
-      </c>
+      <c r="AA82" s="2"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="14" t="str">
@@ -25458,7 +25459,9 @@
       <c r="Z83" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="AA83" s="2"/>
+      <c r="AA83" s="2" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="14" t="str">
@@ -25531,7 +25534,7 @@
         <v>1</v>
       </c>
       <c r="AA84" s="2" t="n">
-        <v>0.2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25585,7 +25588,7 @@
         <v>8.98</v>
       </c>
       <c r="AA85" s="2" t="n">
-        <v>20</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25658,9 +25661,7 @@
       <c r="Z86" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="AA86" s="2" t="n">
-        <v>1.4</v>
-      </c>
+      <c r="AA86" s="2"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="14" t="str">
@@ -25712,7 +25713,9 @@
       <c r="Z87" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="AA87" s="2"/>
+      <c r="AA87" s="2" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="14" t="s">
@@ -25760,9 +25763,6 @@
       <c r="X88" s="8"/>
       <c r="Y88" s="8"/>
       <c r="Z88" s="8"/>
-      <c r="AA88" s="2" t="n">
-        <v>5</v>
-      </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="14" t="str">
@@ -25844,6 +25844,7 @@
       <c r="X91" s="50"/>
       <c r="Y91" s="50"/>
       <c r="Z91" s="50"/>
+      <c r="AA91" s="7"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="14" t="str">
@@ -25917,7 +25918,6 @@
       <c r="Z92" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="AA92" s="7"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="14" t="str">
@@ -26260,6 +26260,10 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="AA97" s="9" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="14" t="str">
@@ -26355,10 +26359,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AA98" s="9" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="AA98" s="9"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="14" t="str">
@@ -26528,7 +26529,9 @@
       <c r="Z100" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="AA100" s="9"/>
+      <c r="AA100" s="8" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="14" t="str">
@@ -26624,9 +26627,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AA101" s="8" t="n">
-        <v>2</v>
-      </c>
+      <c r="AA101" s="9"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="14" t="str">
@@ -26722,7 +26723,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AA102" s="9"/>
+      <c r="AA102" s="8"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="14" t="str">
@@ -26796,7 +26797,9 @@
       <c r="Z103" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="AA103" s="8"/>
+      <c r="AA103" s="8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="14" t="str">
@@ -26892,7 +26895,8 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AA104" s="8" t="n">
+      <c r="AA104" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -26990,7 +26994,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AA105" s="9" t="n">
+      <c r="AA105" s="37" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -27067,9 +27071,8 @@
       <c r="Z106" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="AA106" s="37" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="AA106" s="8" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27094,9 +27097,6 @@
       <c r="X107" s="8"/>
       <c r="Y107" s="8"/>
       <c r="Z107" s="8"/>
-      <c r="AA107" s="8" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="14" t="s">
@@ -27155,7 +27155,7 @@
   </sheetPr>
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E36" activeCellId="0" sqref="E36"/>
     </sheetView>
   </sheetViews>

</xml_diff>